<commit_message>
Counts of desirable CMO operations ~153. I.e. more than 256
</commit_message>
<xml_diff>
--- a/CMOs.xlsx
+++ b/CMOs.xlsx
@@ -8,23 +8,113 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy.glew\Desktop\CMOs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC60613-B92C-4978-B828-744ECC69BE88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B8E008-AB84-467F-84CF-87D73E37E6C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-14630" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Counting" sheetId="2" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andy Glew</author>
+  </authors>
+  <commentList>
+    <comment ref="AK9" authorId="0" shapeId="0" xr:uid="{832B7D08-F99E-4154-8D6D-6C02DDC5C564}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andy Glew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Krste hates me saying "Battery Backed up DRAM" or "NVRAM".  Insufficiently abstract.
+I am OK on defining terms like "Long Term Persistence" - but it sure does help to map those to things the user already knows.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="0" shapeId="0" xr:uid="{67F85F19-AE1C-47E9-B1EF-4D386DB2B46C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andy Glew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Want special privilege for cache locking, whether by line or way.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I29" authorId="0" shapeId="0" xr:uid="{B149EA91-04CF-4DA4-B1AD-DF0479C81967}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andy Glew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Want special privilege for cache locking, whether by line or way.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Andy Glew</author>
@@ -229,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="213">
   <si>
     <t>User Abstract</t>
   </si>
@@ -845,12 +935,140 @@
 I.e. "To" might be a bitmask.
 As also might be "from", in most general sense.</t>
   </si>
+  <si>
+    <t>[I-&gt;Uid)</t>
+  </si>
+  <si>
+    <t>[D-&gt;NVRAM)</t>
+  </si>
+  <si>
+    <t>[D-&gt;Uid*)</t>
+  </si>
+  <si>
+    <t>[D-&gt;Ud*)</t>
+  </si>
+  <si>
+    <t>[D*-&gt;Unc)</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>DISCARD</t>
+  </si>
+  <si>
+    <t>DW (IBM) calls this FLUSH
+Intel - WBINVD</t>
+  </si>
+  <si>
+    <t>Useful NC I/O: FLUSH;I/O;DISCARD
+Security issue</t>
+  </si>
+  <si>
+    <t>DW INVAL.I</t>
+  </si>
+  <si>
+    <t>INVALIDATE CLEAN</t>
+  </si>
+  <si>
+    <t>[D=-&gt;Uio)</t>
+  </si>
+  <si>
+    <t>Useful NC I/O: FLUSH;I/O;INV-C
+Useful SW managed CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AE </t>
+  </si>
+  <si>
+    <t>… + zero mem</t>
+  </si>
+  <si>
+    <t>Zero if found in cache</t>
+  </si>
+  <si>
+    <t>.. + efficient bus zero if not in cache</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x2 Security</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>PREFETCH-X</t>
+  </si>
+  <si>
+    <t>I$&lt;-</t>
+  </si>
+  <si>
+    <t>L1 D$</t>
+  </si>
+  <si>
+    <t>L2 Uid$</t>
+  </si>
+  <si>
+    <t>[M&lt;-NV]</t>
+  </si>
+  <si>
+    <t>L3? Shared $</t>
+  </si>
+  <si>
+    <t>? io</t>
+  </si>
+  <si>
+    <t>Fetch &amp; LOCK</t>
+  </si>
+  <si>
+    <t>Zalloc &amp; LOCK</t>
+  </si>
+  <si>
+    <t>Prefetching into all caches in coherence domain possible, but … TBD
+Prefetching into specified non-local cac hes …
+Prefetching may want to stop at a level, and not allocate in some levels</t>
+  </si>
+  <si>
+    <t>[D-&gt;first NVRAM)</t>
+  </si>
+  <si>
+    <t>[D-&gt;all NVRAM*)</t>
+  </si>
+  <si>
+    <t>count ?AE</t>
+  </si>
+  <si>
+    <t>count AE</t>
+  </si>
+  <si>
+    <t>Total ?AE</t>
+  </si>
+  <si>
+    <t>Total AE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,8 +1186,30 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1004,6 +1244,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor theme="0" tint="-4.9989318521683403E-2"/>
       </patternFill>
     </fill>
   </fills>
@@ -1137,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="45"/>
@@ -1370,15 +1622,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1390,6 +1633,192 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1414,6 +1843,70 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9094</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Elbow 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA9629C3-0BDB-4EFD-887D-C679289E7BB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="0" y="12458700"/>
+          <a:ext cx="12269" cy="423284"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5157,15 +5650,3132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9270FA2A-E9C1-46D1-9859-AA4C05C936C8}">
+  <dimension ref="B4:BR31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="6" ySplit="6" topLeftCell="AL10" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="AP4" sqref="AP1:AP1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9" style="9"/>
+    <col min="2" max="2" width="2.59765625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="3.73046875" style="56" customWidth="1"/>
+    <col min="4" max="4" width="11.06640625" style="56" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="25" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="15" max="18" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="3.59765625" style="19" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="26" max="32" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="3.59765625" style="19" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="3.59765625" style="19" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="3.59765625" style="9" hidden="1" customWidth="1"/>
+    <col min="38" max="40" width="3.59765625" style="9" customWidth="1"/>
+    <col min="41" max="41" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="3.59765625" style="135" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="45" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="3.59765625" style="9" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="3.59765625" style="109" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="60" max="60" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="3.59765625" style="19" customWidth="1"/>
+    <col min="67" max="68" width="3.59765625" style="9" customWidth="1"/>
+    <col min="69" max="69" width="73.265625" style="9" customWidth="1"/>
+    <col min="70" max="70" width="2.59765625" style="9" customWidth="1"/>
+    <col min="71" max="16384" width="9" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:70" outlineLevel="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B5" s="37"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="37"/>
+      <c r="AO5" s="37"/>
+      <c r="AQ5" s="37"/>
+      <c r="AR5" s="37"/>
+      <c r="AS5" s="37"/>
+      <c r="AT5" s="37"/>
+      <c r="AU5" s="37"/>
+      <c r="AW5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="BA5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BG5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BK5" s="37"/>
+      <c r="BM5" s="37"/>
+      <c r="BN5" s="37"/>
+      <c r="BO5" s="37"/>
+      <c r="BP5" s="37"/>
+      <c r="BQ5" s="37"/>
+      <c r="BR5" s="37"/>
+    </row>
+    <row r="6" spans="2:70" ht="25.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="4"/>
+      <c r="C6" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="136"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="89"/>
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="110"/>
+      <c r="AY6" s="11"/>
+      <c r="AZ6" s="89"/>
+      <c r="BA6" s="11"/>
+      <c r="BB6" s="89"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="89"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="89"/>
+      <c r="BG6" s="11"/>
+      <c r="BH6" s="89"/>
+      <c r="BI6" s="11"/>
+      <c r="BJ6" s="89"/>
+      <c r="BK6" s="11"/>
+      <c r="BL6" s="89"/>
+      <c r="BM6" s="11"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="11"/>
+      <c r="BP6" s="11"/>
+      <c r="BQ6" s="11"/>
+      <c r="BR6" s="12"/>
+    </row>
+    <row r="7" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B7" s="4"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="14"/>
+      <c r="AN7" s="14"/>
+      <c r="AO7" s="14"/>
+      <c r="AP7" s="137"/>
+      <c r="AQ7" s="14"/>
+      <c r="AR7" s="14"/>
+      <c r="AS7" s="14"/>
+      <c r="AT7" s="14"/>
+      <c r="AU7" s="14"/>
+      <c r="AV7" s="90"/>
+      <c r="AW7" s="14"/>
+      <c r="AX7" s="111"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="90"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="90"/>
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="90"/>
+      <c r="BE7" s="14"/>
+      <c r="BF7" s="90"/>
+      <c r="BG7" s="14"/>
+      <c r="BH7" s="90"/>
+      <c r="BI7" s="14"/>
+      <c r="BJ7" s="90"/>
+      <c r="BK7" s="14"/>
+      <c r="BL7" s="90"/>
+      <c r="BM7" s="14"/>
+      <c r="BN7" s="13"/>
+      <c r="BO7" s="14"/>
+      <c r="BP7" s="14"/>
+      <c r="BQ7" s="14"/>
+      <c r="BR7" s="12"/>
+    </row>
+    <row r="8" spans="2:70" s="103" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="93"/>
+      <c r="C8" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="99" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="99" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="99" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="99" t="s">
+        <v>140</v>
+      </c>
+      <c r="S8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="U8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="W8" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="X8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z8" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB8" s="99" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE8" s="99" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF8" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI8" s="99"/>
+      <c r="AJ8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL8" s="100" t="s">
+        <v>211</v>
+      </c>
+      <c r="AM8" s="100" t="s">
+        <v>212</v>
+      </c>
+      <c r="AN8" s="100" t="s">
+        <v>195</v>
+      </c>
+      <c r="AO8" s="100" t="s">
+        <v>209</v>
+      </c>
+      <c r="AP8" s="138" t="s">
+        <v>210</v>
+      </c>
+      <c r="AQ8" s="100" t="str">
+        <f xml:space="preserve"> "count " &amp; AQ10</f>
+        <v>count ?</v>
+      </c>
+      <c r="AR8" s="100" t="str">
+        <f t="shared" ref="AR8:AS8" si="0" xml:space="preserve"> "count " &amp; AR10</f>
+        <v>count A</v>
+      </c>
+      <c r="AS8" s="100" t="str">
+        <f t="shared" si="0"/>
+        <v>count E</v>
+      </c>
+      <c r="AT8" s="100"/>
+      <c r="AU8" s="99"/>
+      <c r="AV8" s="104" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW8" s="99"/>
+      <c r="AX8" s="112" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY8" s="99"/>
+      <c r="AZ8" s="104" t="s">
+        <v>175</v>
+      </c>
+      <c r="BA8" s="99"/>
+      <c r="BB8" s="104" t="s">
+        <v>176</v>
+      </c>
+      <c r="BC8" s="99"/>
+      <c r="BD8" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="BE8" s="99"/>
+      <c r="BF8" s="104" t="s">
+        <v>170</v>
+      </c>
+      <c r="BG8" s="99"/>
+      <c r="BH8" s="104" t="s">
+        <v>164</v>
+      </c>
+      <c r="BI8" s="99"/>
+      <c r="BJ8" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="BK8" s="99"/>
+      <c r="BL8" s="104" t="s">
+        <v>208</v>
+      </c>
+      <c r="BM8" s="99"/>
+      <c r="BN8" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO8" s="99"/>
+      <c r="BP8" s="99"/>
+      <c r="BQ8" s="95"/>
+      <c r="BR8" s="102"/>
+    </row>
+    <row r="9" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B9" s="4"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="84"/>
+      <c r="Z9" s="85"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="85"/>
+      <c r="AC9" s="85"/>
+      <c r="AD9" s="85"/>
+      <c r="AE9" s="85"/>
+      <c r="AF9" s="86"/>
+      <c r="AG9" s="42"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="42"/>
+      <c r="AJ9" s="42"/>
+      <c r="AK9" s="76"/>
+      <c r="AL9" s="77"/>
+      <c r="AM9" s="77"/>
+      <c r="AN9" s="77"/>
+      <c r="AO9" s="77"/>
+      <c r="AP9" s="139"/>
+      <c r="AQ9" s="77"/>
+      <c r="AR9" s="77"/>
+      <c r="AS9" s="77"/>
+      <c r="AT9" s="77"/>
+      <c r="AU9" s="77"/>
+      <c r="AV9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="AW9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX9" s="113" t="s">
+        <v>178</v>
+      </c>
+      <c r="AY9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BA9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BB9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BC9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BD9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BF9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BG9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BH9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BJ9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BK9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL9" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BM9" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BN9" s="42"/>
+      <c r="BO9" s="42"/>
+      <c r="BP9" s="42"/>
+      <c r="BQ9" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="BR9" s="12"/>
+    </row>
+    <row r="10" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B10" s="37"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38"/>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="38"/>
+      <c r="AL10" s="38"/>
+      <c r="AM10" s="38"/>
+      <c r="AN10" s="38"/>
+      <c r="AO10" s="38"/>
+      <c r="AP10" s="140"/>
+      <c r="AQ10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR10" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS10" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT10" s="38"/>
+      <c r="AU10" s="38"/>
+      <c r="AV10" s="92"/>
+      <c r="AW10" s="38"/>
+      <c r="AX10" s="114"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="92"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="92"/>
+      <c r="BC10" s="38"/>
+      <c r="BD10" s="92"/>
+      <c r="BE10" s="38"/>
+      <c r="BF10" s="92"/>
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="92"/>
+      <c r="BI10" s="38"/>
+      <c r="BJ10" s="92"/>
+      <c r="BK10" s="38"/>
+      <c r="BL10" s="92"/>
+      <c r="BM10" s="38"/>
+      <c r="BN10" s="38"/>
+      <c r="BO10" s="38"/>
+      <c r="BP10" s="38"/>
+      <c r="BQ10" s="38"/>
+      <c r="BR10" s="37"/>
+    </row>
+    <row r="11" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B11" s="37"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="38"/>
+      <c r="AJ11" s="38"/>
+      <c r="AK11" s="38"/>
+      <c r="AL11" s="38">
+        <f>SUM(AL13:AL20)</f>
+        <v>153</v>
+      </c>
+      <c r="AM11" s="38">
+        <f>SUM(AM13:AM20)</f>
+        <v>137</v>
+      </c>
+      <c r="AN11" s="38"/>
+      <c r="AO11" s="38"/>
+      <c r="AP11" s="140"/>
+      <c r="AQ11" s="38"/>
+      <c r="AR11" s="38"/>
+      <c r="AS11" s="38"/>
+      <c r="AT11" s="38"/>
+      <c r="AU11" s="38"/>
+      <c r="AV11" s="92"/>
+      <c r="AW11" s="38"/>
+      <c r="AX11" s="114"/>
+      <c r="AY11" s="38"/>
+      <c r="AZ11" s="92"/>
+      <c r="BA11" s="38"/>
+      <c r="BB11" s="92"/>
+      <c r="BC11" s="38"/>
+      <c r="BD11" s="92"/>
+      <c r="BE11" s="38"/>
+      <c r="BF11" s="92"/>
+      <c r="BG11" s="38"/>
+      <c r="BH11" s="92"/>
+      <c r="BI11" s="38"/>
+      <c r="BJ11" s="92"/>
+      <c r="BK11" s="38"/>
+      <c r="BL11" s="92"/>
+      <c r="BM11" s="38"/>
+      <c r="BN11" s="38"/>
+      <c r="BO11" s="38"/>
+      <c r="BP11" s="38"/>
+      <c r="BQ11" s="38"/>
+      <c r="BR11" s="37"/>
+    </row>
+    <row r="12" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B12" s="37"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38"/>
+      <c r="AI12" s="38"/>
+      <c r="AJ12" s="38"/>
+      <c r="AK12" s="38"/>
+      <c r="AL12" s="38"/>
+      <c r="AM12" s="38"/>
+      <c r="AN12" s="38"/>
+      <c r="AO12" s="38"/>
+      <c r="AP12" s="140"/>
+      <c r="AQ12" s="38"/>
+      <c r="AR12" s="38"/>
+      <c r="AS12" s="38"/>
+      <c r="AT12" s="38"/>
+      <c r="AU12" s="38"/>
+      <c r="AV12" s="92"/>
+      <c r="AW12" s="38"/>
+      <c r="AX12" s="114"/>
+      <c r="AY12" s="38"/>
+      <c r="AZ12" s="92"/>
+      <c r="BA12" s="38"/>
+      <c r="BB12" s="92"/>
+      <c r="BC12" s="38"/>
+      <c r="BD12" s="92"/>
+      <c r="BE12" s="38"/>
+      <c r="BF12" s="92"/>
+      <c r="BG12" s="38"/>
+      <c r="BH12" s="92"/>
+      <c r="BI12" s="38"/>
+      <c r="BJ12" s="92"/>
+      <c r="BK12" s="38"/>
+      <c r="BL12" s="92"/>
+      <c r="BM12" s="38"/>
+      <c r="BN12" s="38"/>
+      <c r="BO12" s="38"/>
+      <c r="BP12" s="38"/>
+      <c r="BQ12" s="38"/>
+      <c r="BR12" s="37"/>
+    </row>
+    <row r="13" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="4"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="16"/>
+      <c r="N13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="16"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="7"/>
+      <c r="AL13" s="7">
+        <f>AN13*AO13:AO14</f>
+        <v>32</v>
+      </c>
+      <c r="AM13" s="7">
+        <f>AN13*AP13</f>
+        <v>32</v>
+      </c>
+      <c r="AN13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="7">
+        <f>SUM(AQ13:AS13)</f>
+        <v>32</v>
+      </c>
+      <c r="AP13" s="140">
+        <f>SUM(AR13:AS13)</f>
+        <v>32</v>
+      </c>
+      <c r="AQ13" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV13:$BM13)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AR13" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV13:$BM13)))))</f>
+        <v>16</v>
+      </c>
+      <c r="AS13" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV13:$BM13)))))</f>
+        <v>16</v>
+      </c>
+      <c r="AT13" s="7"/>
+      <c r="AU13" s="7"/>
+      <c r="AV13" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW13" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX13" s="115" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY13" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AZ13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BA13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BB13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BH13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BI13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BK13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM13" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN13" s="16"/>
+      <c r="BO13" s="7"/>
+      <c r="BP13" s="7"/>
+      <c r="BQ13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="BR13" s="12"/>
+    </row>
+    <row r="14" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="4"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="16"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="16"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="16"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7">
+        <f t="shared" ref="AL14:AL20" si="1">AN14*AO14:AO15</f>
+        <v>64</v>
+      </c>
+      <c r="AM14" s="7">
+        <f t="shared" ref="AM14:AM20" si="2">AN14*AP14</f>
+        <v>64</v>
+      </c>
+      <c r="AN14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AO14" s="7">
+        <f t="shared" ref="AO14:AO20" si="3">SUM(AQ14:AS14)</f>
+        <v>32</v>
+      </c>
+      <c r="AP14" s="140">
+        <f t="shared" ref="AP14:AP20" si="4">SUM(AR14:AS14)</f>
+        <v>32</v>
+      </c>
+      <c r="AQ14" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV14:$BM14)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AR14" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV14:$BM14)))))</f>
+        <v>16</v>
+      </c>
+      <c r="AS14" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV14:$BM14)))))</f>
+        <v>16</v>
+      </c>
+      <c r="AT14" s="7"/>
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW14" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX14" s="115" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY14" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AZ14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BA14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BB14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BH14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BI14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BK14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN14" s="16"/>
+      <c r="BO14" s="7"/>
+      <c r="BP14" s="7"/>
+      <c r="BQ14" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="BR14" s="12"/>
+    </row>
+    <row r="15" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="4"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AM15" s="7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AO15" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AP15" s="140">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AQ15" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV15:$BM15)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AR15" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV15:$BM15)))))</f>
+        <v>1</v>
+      </c>
+      <c r="AS15" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV15:$BM15)))))</f>
+        <v>1</v>
+      </c>
+      <c r="AT15" s="7"/>
+      <c r="AU15" s="7"/>
+      <c r="AV15" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX15" s="114" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AZ15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BB15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BL15" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM15" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN15" s="16"/>
+      <c r="BO15" s="7"/>
+      <c r="BP15" s="7"/>
+      <c r="BQ15" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="BR15" s="12"/>
+    </row>
+    <row r="16" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="4"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="108" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="106" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="16"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="AM16" s="7">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AN16" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="7">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="AP16" s="140">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="AQ16" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV16:$BM16)))))</f>
+        <v>8</v>
+      </c>
+      <c r="AR16" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV16:$BM16)))))</f>
+        <v>6</v>
+      </c>
+      <c r="AS16" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV16:$BM16)))))</f>
+        <v>6</v>
+      </c>
+      <c r="AT16" s="7"/>
+      <c r="AU16" s="7"/>
+      <c r="AV16" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW16" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX16" s="115" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY16" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AZ16" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BB16" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC16" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD16" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE16" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF16" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="BG16" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="BH16" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BJ16" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BK16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BL16" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BN16" s="16"/>
+      <c r="BO16" s="7"/>
+      <c r="BP16" s="7"/>
+      <c r="BQ16" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="BR16" s="12"/>
+    </row>
+    <row r="17" spans="2:70" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="4"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="107" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="16"/>
+      <c r="N17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U17" s="16"/>
+      <c r="V17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="75"/>
+      <c r="Z17" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="7"/>
+      <c r="AL17" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AM17" s="7">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AN17" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="7">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="AP17" s="140">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AQ17" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV17:$BM17)))))</f>
+        <v>8</v>
+      </c>
+      <c r="AR17" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV17:$BM17)))))</f>
+        <v>4</v>
+      </c>
+      <c r="AS17" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV17:$BM17)))))</f>
+        <v>4</v>
+      </c>
+      <c r="AT17" s="7"/>
+      <c r="AU17" s="7"/>
+      <c r="AV17" s="92"/>
+      <c r="AW17" s="7"/>
+      <c r="AX17" s="114"/>
+      <c r="AY17" s="7"/>
+      <c r="AZ17" s="92"/>
+      <c r="BA17" s="7"/>
+      <c r="BB17" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC17" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD17" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE17" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF17" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH17" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BJ17" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BK17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BL17" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BN17" s="16"/>
+      <c r="BO17" s="7"/>
+      <c r="BP17" s="7"/>
+      <c r="BQ17" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="BR17" s="12"/>
+    </row>
+    <row r="18" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="4"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="16"/>
+      <c r="N18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" s="16"/>
+      <c r="V18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC18" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD18" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF18" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG18" s="16"/>
+      <c r="AH18" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="16"/>
+      <c r="AK18" s="7"/>
+      <c r="AL18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM18" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN18" s="7"/>
+      <c r="AO18" s="7">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="AP18" s="140">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV18:$BM18)))))</f>
+        <v>12</v>
+      </c>
+      <c r="AR18" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV18:$BM18)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AS18" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV18:$BM18)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AT18" s="7"/>
+      <c r="AU18" s="7"/>
+      <c r="AV18" s="92"/>
+      <c r="AW18" s="7"/>
+      <c r="AX18" s="114"/>
+      <c r="AY18" s="7"/>
+      <c r="AZ18" s="92"/>
+      <c r="BA18" s="7"/>
+      <c r="BB18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BC18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BD18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BE18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BF18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BJ18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BK18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BL18" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BN18" s="16"/>
+      <c r="BO18" s="7"/>
+      <c r="BP18" s="7"/>
+      <c r="BQ18" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="BR18" s="8"/>
+    </row>
+    <row r="19" spans="2:70" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="4"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="U19" s="16"/>
+      <c r="V19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="75"/>
+      <c r="Z19" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA19" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB19" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC19" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD19" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE19" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF19" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="7"/>
+      <c r="AL19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM19" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN19" s="7"/>
+      <c r="AO19" s="7">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="AP19" s="140">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV19:$BM19)))))</f>
+        <v>12</v>
+      </c>
+      <c r="AR19" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV19:$BM19)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AS19" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV19:$BM19)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AT19" s="7"/>
+      <c r="AU19" s="7"/>
+      <c r="AV19" s="92"/>
+      <c r="AW19" s="7"/>
+      <c r="AX19" s="114"/>
+      <c r="AY19" s="7"/>
+      <c r="AZ19" s="92"/>
+      <c r="BA19" s="7"/>
+      <c r="BB19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BC19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BD19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BE19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BF19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BJ19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BK19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BL19" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BN19" s="16"/>
+      <c r="BO19" s="7"/>
+      <c r="BP19" s="7"/>
+      <c r="BQ19" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="BR19" s="8"/>
+    </row>
+    <row r="20" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="4"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="U20" s="16"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="7"/>
+      <c r="AL20" s="7">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="AM20" s="7">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="AN20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="7">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="AP20" s="140">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="AQ20" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV20:$BM20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AR20" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV20:$BM20)))))</f>
+        <v>17</v>
+      </c>
+      <c r="AS20" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV20:$BM20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="AT20" s="7"/>
+      <c r="AU20" s="7"/>
+      <c r="AV20" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW20" s="7"/>
+      <c r="AX20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AZ20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BB20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BD20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BE20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BF20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BG20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BJ20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BL20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BN20" s="16"/>
+      <c r="BO20" s="7"/>
+      <c r="BP20" s="7"/>
+      <c r="BQ20" s="18"/>
+      <c r="BR20" s="12"/>
+    </row>
+    <row r="21" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B21" s="37"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38"/>
+      <c r="AJ21" s="38"/>
+      <c r="AK21" s="38"/>
+      <c r="AL21" s="38"/>
+      <c r="AM21" s="38"/>
+      <c r="AN21" s="38"/>
+      <c r="AO21" s="38"/>
+      <c r="AP21" s="140"/>
+      <c r="AQ21" s="38"/>
+      <c r="AR21" s="38"/>
+      <c r="AS21" s="38"/>
+      <c r="AT21" s="38"/>
+      <c r="AU21" s="38"/>
+      <c r="AV21" s="92"/>
+      <c r="AW21" s="38"/>
+      <c r="AX21" s="114"/>
+      <c r="AY21" s="38"/>
+      <c r="AZ21" s="92"/>
+      <c r="BA21" s="38"/>
+      <c r="BB21" s="92"/>
+      <c r="BC21" s="38"/>
+      <c r="BD21" s="92"/>
+      <c r="BE21" s="38"/>
+      <c r="BF21" s="92"/>
+      <c r="BG21" s="38"/>
+      <c r="BH21" s="92"/>
+      <c r="BI21" s="38"/>
+      <c r="BJ21" s="92"/>
+      <c r="BK21" s="38"/>
+      <c r="BL21" s="92"/>
+      <c r="BM21" s="38"/>
+      <c r="BN21" s="38"/>
+      <c r="BO21" s="38"/>
+      <c r="BP21" s="38"/>
+      <c r="BQ21" s="38"/>
+      <c r="BR21" s="37"/>
+    </row>
+    <row r="22" spans="2:70" s="103" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="93"/>
+      <c r="C22" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" s="99" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="99" t="s">
+        <v>137</v>
+      </c>
+      <c r="P22" s="99" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q22" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="R22" s="99" t="s">
+        <v>140</v>
+      </c>
+      <c r="S22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="T22" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="U22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="V22" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="W22" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="X22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z22" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA22" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB22" s="99" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC22" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD22" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE22" s="99" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF22" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI22" s="99"/>
+      <c r="AJ22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL22" s="100"/>
+      <c r="AM22" s="100" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN22" s="100"/>
+      <c r="AO22" s="100"/>
+      <c r="AP22" s="138"/>
+      <c r="AQ22" s="100"/>
+      <c r="AR22" s="100"/>
+      <c r="AS22" s="100"/>
+      <c r="AT22" s="100"/>
+      <c r="AU22" s="99"/>
+      <c r="AV22" s="104" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW22" s="99"/>
+      <c r="AX22" s="112" t="s">
+        <v>199</v>
+      </c>
+      <c r="AY22" s="99"/>
+      <c r="AZ22" s="104" t="s">
+        <v>200</v>
+      </c>
+      <c r="BA22" s="99"/>
+      <c r="BB22" s="104" t="s">
+        <v>202</v>
+      </c>
+      <c r="BC22" s="99"/>
+      <c r="BD22" s="104" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE22" s="99"/>
+      <c r="BF22" s="104" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG22" s="99"/>
+      <c r="BH22" s="104"/>
+      <c r="BI22" s="99"/>
+      <c r="BJ22" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="BK22" s="99"/>
+      <c r="BL22" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="BM22" s="99"/>
+      <c r="BN22" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO22" s="99"/>
+      <c r="BP22" s="99"/>
+      <c r="BQ22" s="95"/>
+      <c r="BR22" s="102"/>
+    </row>
+    <row r="23" spans="2:70" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B23" s="37"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="117"/>
+      <c r="O23" s="117"/>
+      <c r="P23" s="117"/>
+      <c r="Q23" s="117"/>
+      <c r="R23" s="117"/>
+      <c r="S23" s="117"/>
+      <c r="T23" s="117"/>
+      <c r="U23" s="117"/>
+      <c r="V23" s="117"/>
+      <c r="W23" s="117"/>
+      <c r="X23" s="117"/>
+      <c r="Y23" s="117"/>
+      <c r="Z23" s="117"/>
+      <c r="AA23" s="117"/>
+      <c r="AB23" s="117"/>
+      <c r="AC23" s="117"/>
+      <c r="AD23" s="117"/>
+      <c r="AE23" s="117"/>
+      <c r="AF23" s="117"/>
+      <c r="AG23" s="117"/>
+      <c r="AH23" s="117"/>
+      <c r="AI23" s="117"/>
+      <c r="AJ23" s="117"/>
+      <c r="AK23" s="117"/>
+      <c r="AL23" s="117"/>
+      <c r="AM23" s="117"/>
+      <c r="AN23" s="117"/>
+      <c r="AO23" s="117"/>
+      <c r="AP23" s="141"/>
+      <c r="AQ23" s="117"/>
+      <c r="AR23" s="117"/>
+      <c r="AS23" s="117"/>
+      <c r="AT23" s="117"/>
+      <c r="AU23" s="117"/>
+      <c r="AV23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="AW23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX23" s="113" t="s">
+        <v>178</v>
+      </c>
+      <c r="AY23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BA23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BB23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BC23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BD23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BF23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BG23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BH23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BJ23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BK23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL23" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="BM23" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="BN23" s="38"/>
+      <c r="BO23" s="38"/>
+      <c r="BP23" s="38"/>
+      <c r="BQ23" s="122" t="s">
+        <v>206</v>
+      </c>
+      <c r="BR23" s="37"/>
+    </row>
+    <row r="24" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B24" s="37"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+      <c r="AA24" s="18"/>
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="18"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="18"/>
+      <c r="AG24" s="18"/>
+      <c r="AH24" s="18"/>
+      <c r="AI24" s="18"/>
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+      <c r="AL24" s="18"/>
+      <c r="AM24" s="18"/>
+      <c r="AN24" s="18"/>
+      <c r="AO24" s="18"/>
+      <c r="AP24" s="142"/>
+      <c r="AQ24" s="18"/>
+      <c r="AR24" s="18"/>
+      <c r="AS24" s="18"/>
+      <c r="AT24" s="18"/>
+      <c r="AU24" s="18"/>
+      <c r="AV24" s="92"/>
+      <c r="AW24" s="7"/>
+      <c r="AX24" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ24" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB24" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD24" s="92"/>
+      <c r="BE24" s="7"/>
+      <c r="BF24" s="92"/>
+      <c r="BG24" s="7"/>
+      <c r="BH24" s="92"/>
+      <c r="BI24" s="7"/>
+      <c r="BJ24" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL24" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN24" s="38"/>
+      <c r="BO24" s="38"/>
+      <c r="BP24" s="38"/>
+      <c r="BQ24" s="18"/>
+      <c r="BR24" s="37"/>
+    </row>
+    <row r="25" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B25" s="37"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="18"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="18"/>
+      <c r="AM25" s="18"/>
+      <c r="AN25" s="18"/>
+      <c r="AO25" s="18"/>
+      <c r="AP25" s="142"/>
+      <c r="AQ25" s="18"/>
+      <c r="AR25" s="18"/>
+      <c r="AS25" s="18"/>
+      <c r="AT25" s="18"/>
+      <c r="AU25" s="18"/>
+      <c r="AV25" s="92"/>
+      <c r="AW25" s="7"/>
+      <c r="AX25" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ25" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB25" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD25" s="92"/>
+      <c r="BE25" s="7"/>
+      <c r="BF25" s="92"/>
+      <c r="BG25" s="7"/>
+      <c r="BH25" s="92"/>
+      <c r="BI25" s="7"/>
+      <c r="BJ25" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL25" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="BM25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN25" s="38"/>
+      <c r="BO25" s="38"/>
+      <c r="BP25" s="38"/>
+      <c r="BQ25" s="18"/>
+      <c r="BR25" s="37"/>
+    </row>
+    <row r="26" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B26" s="37"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="18"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="18"/>
+      <c r="AM26" s="18"/>
+      <c r="AN26" s="18"/>
+      <c r="AO26" s="18"/>
+      <c r="AP26" s="142"/>
+      <c r="AQ26" s="18"/>
+      <c r="AR26" s="18"/>
+      <c r="AS26" s="18"/>
+      <c r="AT26" s="18"/>
+      <c r="AU26" s="18"/>
+      <c r="AV26" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX26" s="92"/>
+      <c r="AY26" s="7"/>
+      <c r="AZ26" s="92"/>
+      <c r="BA26" s="7"/>
+      <c r="BB26" s="92"/>
+      <c r="BC26" s="7"/>
+      <c r="BD26" s="92"/>
+      <c r="BE26" s="7"/>
+      <c r="BF26" s="92"/>
+      <c r="BG26" s="7"/>
+      <c r="BH26" s="92"/>
+      <c r="BI26" s="7"/>
+      <c r="BJ26" s="92"/>
+      <c r="BK26" s="7"/>
+      <c r="BL26" s="92"/>
+      <c r="BM26" s="7"/>
+      <c r="BN26" s="38"/>
+      <c r="BO26" s="38"/>
+      <c r="BP26" s="38"/>
+      <c r="BQ26" s="18"/>
+      <c r="BR26" s="37"/>
+    </row>
+    <row r="27" spans="2:70" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="4"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="16"/>
+      <c r="N27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="16"/>
+      <c r="V27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W27" s="7"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF27" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG27" s="16"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="7"/>
+      <c r="AL27" s="7"/>
+      <c r="AM27" s="7"/>
+      <c r="AN27" s="7"/>
+      <c r="AO27" s="7"/>
+      <c r="AP27" s="140"/>
+      <c r="AQ27" s="7"/>
+      <c r="AR27" s="7"/>
+      <c r="AS27" s="7"/>
+      <c r="AT27" s="7"/>
+      <c r="AU27" s="7"/>
+      <c r="AV27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD27" s="92"/>
+      <c r="BE27" s="7"/>
+      <c r="BF27" s="92"/>
+      <c r="BG27" s="7"/>
+      <c r="BH27" s="92"/>
+      <c r="BI27" s="7"/>
+      <c r="BJ27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL27" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN27" s="16"/>
+      <c r="BO27" s="7"/>
+      <c r="BP27" s="7"/>
+      <c r="BQ27" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="BR27" s="12"/>
+    </row>
+    <row r="28" spans="2:70" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="4"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="45"/>
+      <c r="AB28" s="45"/>
+      <c r="AC28" s="45"/>
+      <c r="AD28" s="45"/>
+      <c r="AE28" s="45"/>
+      <c r="AF28" s="45"/>
+      <c r="AG28" s="16"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="7"/>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="7"/>
+      <c r="AL28" s="7"/>
+      <c r="AM28" s="7"/>
+      <c r="AN28" s="7"/>
+      <c r="AO28" s="7"/>
+      <c r="AP28" s="140"/>
+      <c r="AQ28" s="7"/>
+      <c r="AR28" s="7"/>
+      <c r="AS28" s="7"/>
+      <c r="AT28" s="7"/>
+      <c r="AU28" s="7"/>
+      <c r="AV28" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX28" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ28" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB28" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD28" s="92"/>
+      <c r="BE28" s="7"/>
+      <c r="BF28" s="92"/>
+      <c r="BG28" s="7"/>
+      <c r="BH28" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ28" s="92"/>
+      <c r="BK28" s="7"/>
+      <c r="BL28" s="92"/>
+      <c r="BM28" s="7"/>
+      <c r="BN28" s="16"/>
+      <c r="BO28" s="7"/>
+      <c r="BP28" s="7"/>
+      <c r="BQ28" s="18"/>
+      <c r="BR28" s="8"/>
+    </row>
+    <row r="29" spans="2:70" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="92" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" s="92"/>
+      <c r="K29" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="92" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="92"/>
+      <c r="N29" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="O29" s="92"/>
+      <c r="P29" s="92"/>
+      <c r="Q29" s="92"/>
+      <c r="R29" s="92"/>
+      <c r="S29" s="92"/>
+      <c r="T29" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="U29" s="92"/>
+      <c r="V29" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="W29" s="92"/>
+      <c r="X29" s="92"/>
+      <c r="Y29" s="92"/>
+      <c r="Z29" s="92" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF29" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG29" s="92"/>
+      <c r="AH29" s="92"/>
+      <c r="AI29" s="92"/>
+      <c r="AJ29" s="92"/>
+      <c r="AK29" s="92"/>
+      <c r="AL29" s="92"/>
+      <c r="AM29" s="92"/>
+      <c r="AN29" s="92"/>
+      <c r="AO29" s="92"/>
+      <c r="AP29" s="140"/>
+      <c r="AQ29" s="92"/>
+      <c r="AR29" s="92"/>
+      <c r="AS29" s="92"/>
+      <c r="AT29" s="92"/>
+      <c r="AU29" s="92"/>
+      <c r="AV29" s="92"/>
+      <c r="AW29" s="92"/>
+      <c r="AX29" s="114"/>
+      <c r="AY29" s="92"/>
+      <c r="AZ29" s="92"/>
+      <c r="BA29" s="92"/>
+      <c r="BB29" s="92"/>
+      <c r="BC29" s="92"/>
+      <c r="BD29" s="92"/>
+      <c r="BE29" s="92"/>
+      <c r="BF29" s="92"/>
+      <c r="BG29" s="92"/>
+      <c r="BH29" s="92"/>
+      <c r="BI29" s="92"/>
+      <c r="BJ29" s="92"/>
+      <c r="BK29" s="92"/>
+      <c r="BL29" s="92"/>
+      <c r="BM29" s="92"/>
+      <c r="BN29" s="92"/>
+      <c r="BO29" s="92"/>
+      <c r="BP29" s="92"/>
+      <c r="BQ29" s="120" t="s">
+        <v>117</v>
+      </c>
+      <c r="BR29" s="90"/>
+    </row>
+    <row r="30" spans="2:70" x14ac:dyDescent="0.45">
+      <c r="B30" s="37"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="38"/>
+      <c r="X30" s="38"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="38"/>
+      <c r="AB30" s="38"/>
+      <c r="AC30" s="38"/>
+      <c r="AD30" s="38"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="38"/>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="38"/>
+      <c r="AI30" s="38"/>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="38"/>
+      <c r="AL30" s="38"/>
+      <c r="AM30" s="38"/>
+      <c r="AN30" s="38"/>
+      <c r="AO30" s="38"/>
+      <c r="AP30" s="140"/>
+      <c r="AQ30" s="38"/>
+      <c r="AR30" s="38"/>
+      <c r="AS30" s="38"/>
+      <c r="AT30" s="38"/>
+      <c r="AU30" s="38"/>
+      <c r="AV30" s="92"/>
+      <c r="AW30" s="38"/>
+      <c r="AX30" s="114"/>
+      <c r="AY30" s="38"/>
+      <c r="AZ30" s="92"/>
+      <c r="BA30" s="38"/>
+      <c r="BB30" s="92"/>
+      <c r="BC30" s="38"/>
+      <c r="BD30" s="92"/>
+      <c r="BE30" s="38"/>
+      <c r="BF30" s="92"/>
+      <c r="BG30" s="38"/>
+      <c r="BH30" s="92"/>
+      <c r="BI30" s="38"/>
+      <c r="BJ30" s="92"/>
+      <c r="BK30" s="38"/>
+      <c r="BL30" s="92"/>
+      <c r="BM30" s="38"/>
+      <c r="BN30" s="38"/>
+      <c r="BO30" s="38"/>
+      <c r="BP30" s="38"/>
+      <c r="BQ30" s="38"/>
+      <c r="BR30" s="37"/>
+    </row>
+    <row r="31" spans="2:70" s="134" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="123"/>
+      <c r="C31" s="124" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="124"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="128" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="128" t="s">
+        <v>76</v>
+      </c>
+      <c r="L31" s="128" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="128" t="s">
+        <v>137</v>
+      </c>
+      <c r="P31" s="128" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q31" s="128" t="s">
+        <v>139</v>
+      </c>
+      <c r="R31" s="128" t="s">
+        <v>140</v>
+      </c>
+      <c r="S31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" s="128" t="s">
+        <v>24</v>
+      </c>
+      <c r="U31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="V31" s="128" t="s">
+        <v>61</v>
+      </c>
+      <c r="W31" s="128" t="s">
+        <v>70</v>
+      </c>
+      <c r="X31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="129" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z31" s="128" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA31" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB31" s="128" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC31" s="128" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD31" s="128" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE31" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF31" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="130" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI31" s="128"/>
+      <c r="AJ31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL31" s="129"/>
+      <c r="AM31" s="129" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN31" s="129" t="s">
+        <v>195</v>
+      </c>
+      <c r="AO31" s="129"/>
+      <c r="AP31" s="143"/>
+      <c r="AQ31" s="129"/>
+      <c r="AR31" s="129"/>
+      <c r="AS31" s="129"/>
+      <c r="AT31" s="129"/>
+      <c r="AU31" s="128"/>
+      <c r="AV31" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW31" s="128"/>
+      <c r="AX31" s="132" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY31" s="128"/>
+      <c r="AZ31" s="131" t="s">
+        <v>175</v>
+      </c>
+      <c r="BA31" s="128"/>
+      <c r="BB31" s="131" t="s">
+        <v>176</v>
+      </c>
+      <c r="BC31" s="128"/>
+      <c r="BD31" s="131" t="s">
+        <v>187</v>
+      </c>
+      <c r="BE31" s="128"/>
+      <c r="BF31" s="131" t="s">
+        <v>170</v>
+      </c>
+      <c r="BG31" s="128"/>
+      <c r="BH31" s="131" t="s">
+        <v>164</v>
+      </c>
+      <c r="BI31" s="128"/>
+      <c r="BJ31" s="131" t="s">
+        <v>173</v>
+      </c>
+      <c r="BK31" s="128"/>
+      <c r="BL31" s="131" t="s">
+        <v>173</v>
+      </c>
+      <c r="BM31" s="128"/>
+      <c r="BN31" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO31" s="128"/>
+      <c r="BP31" s="128"/>
+      <c r="BQ31" s="125"/>
+      <c r="BR31" s="133"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Y9:AF9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:AZ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F72" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="AI74" sqref="AI74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
@@ -5369,7 +8979,7 @@
       </c>
       <c r="D8" s="57"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="81" t="s">
         <v>147</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -5522,14 +9132,14 @@
       <c r="U9" s="42"/>
       <c r="V9" s="42"/>
       <c r="W9" s="42"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="77"/>
-      <c r="Z9" s="77"/>
-      <c r="AA9" s="77"/>
-      <c r="AB9" s="77"/>
-      <c r="AC9" s="77"/>
-      <c r="AD9" s="77"/>
-      <c r="AE9" s="78"/>
+      <c r="X9" s="84"/>
+      <c r="Y9" s="85"/>
+      <c r="Z9" s="85"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="85"/>
+      <c r="AC9" s="85"/>
+      <c r="AD9" s="85"/>
+      <c r="AE9" s="86"/>
       <c r="AF9" s="42"/>
       <c r="AG9" s="43"/>
       <c r="AH9" s="42"/>
@@ -5611,18 +9221,18 @@
     </row>
     <row r="11" spans="2:52" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B11" s="4"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="6" t="s">
         <v>132</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="82"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="67"/>
-      <c r="I11" s="82"/>
+      <c r="I11" s="79"/>
       <c r="J11" s="67"/>
       <c r="K11" s="67"/>
-      <c r="L11" s="82"/>
+      <c r="L11" s="79"/>
       <c r="M11" s="67" t="s">
         <v>134</v>
       </c>
@@ -5630,14 +9240,14 @@
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
       <c r="Q11" s="67"/>
-      <c r="R11" s="82"/>
+      <c r="R11" s="79"/>
       <c r="S11" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="T11" s="82"/>
+      <c r="T11" s="79"/>
       <c r="U11" s="67"/>
       <c r="V11" s="67"/>
-      <c r="W11" s="82"/>
+      <c r="W11" s="79"/>
       <c r="X11" s="67"/>
       <c r="Y11" s="67"/>
       <c r="Z11" s="67"/>
@@ -5648,10 +9258,10 @@
       <c r="AE11" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="AF11" s="82"/>
-      <c r="AG11" s="83"/>
+      <c r="AF11" s="79"/>
+      <c r="AG11" s="80"/>
       <c r="AH11" s="67"/>
-      <c r="AI11" s="82"/>
+      <c r="AI11" s="79"/>
       <c r="AJ11" s="67" t="s">
         <v>135</v>
       </c>
@@ -5667,7 +9277,7 @@
       <c r="AT11" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="AU11" s="82"/>
+      <c r="AU11" s="79"/>
       <c r="AV11" s="67"/>
       <c r="AW11" s="67"/>
       <c r="AX11" s="15"/>
@@ -8166,7 +11776,7 @@
       <c r="AV42" s="26"/>
       <c r="AW42" s="26"/>
       <c r="AX42" s="72"/>
-      <c r="AY42" s="79" t="s">
+      <c r="AY42" s="82" t="s">
         <v>36</v>
       </c>
       <c r="AZ42" s="12"/>
@@ -8260,7 +11870,7 @@
       <c r="AV43" s="26"/>
       <c r="AW43" s="26"/>
       <c r="AX43" s="73"/>
-      <c r="AY43" s="80"/>
+      <c r="AY43" s="83"/>
       <c r="AZ43" s="12"/>
     </row>
     <row r="44" spans="2:52" ht="28.5" outlineLevel="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
late checkin: CMOs.xlsx as of June 10, 2020, 14:43
</commit_message>
<xml_diff>
--- a/CMOs.xlsx
+++ b/CMOs.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy.glew\Desktop\CMOs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glew\Desktop\CMOs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B8E008-AB84-467F-84CF-87D73E37E6C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FB33B8E-00E0-4893-8215-B053E88E7940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-14630" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="-19452" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counting" sheetId="2" r:id="rId1"/>
     <sheet name="Original" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -319,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="213">
   <si>
     <t>User Abstract</t>
   </si>
@@ -1011,9 +1014,6 @@
     <t>x2 Security</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>PREFETCH-X</t>
   </si>
   <si>
@@ -1058,10 +1058,13 @@
     <t>count AE</t>
   </si>
   <si>
-    <t>Total ?AE</t>
-  </si>
-  <si>
-    <t>Total AE</t>
+    <t>set LRU</t>
+  </si>
+  <si>
+    <t>A-only</t>
+  </si>
+  <si>
+    <t>w/o level</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="45"/>
@@ -1634,19 +1637,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1819,6 +1810,21 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5651,76 +5657,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9270FA2A-E9C1-46D1-9859-AA4C05C936C8}">
-  <dimension ref="B4:BR31"/>
+  <dimension ref="B4:BS31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="6" ySplit="6" topLeftCell="AL10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AP4" sqref="AP1:AP1048576"/>
+      <selection pane="bottomRight" activeCell="AO13" sqref="AO13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="9" style="9"/>
-    <col min="2" max="2" width="2.59765625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="3.73046875" style="56" customWidth="1"/>
-    <col min="4" max="4" width="11.06640625" style="56" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="2.578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="3.734375" style="56" customWidth="1"/>
+    <col min="4" max="4" width="11.05078125" style="56" customWidth="1"/>
+    <col min="5" max="5" width="25.3125" style="9" customWidth="1"/>
     <col min="6" max="6" width="25" style="9" customWidth="1"/>
     <col min="7" max="7" width="25" style="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="15" max="18" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="3.59765625" style="19" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="22" max="23" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="26" max="32" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="3.59765625" style="19" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="3.59765625" style="19" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="3.59765625" style="9" hidden="1" customWidth="1"/>
-    <col min="38" max="40" width="3.59765625" style="9" customWidth="1"/>
-    <col min="41" max="41" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="3.59765625" style="135" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="45" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="3.59765625" style="9" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="3.59765625" style="109" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="60" max="60" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="3.59765625" style="88" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="3.59765625" style="19" customWidth="1"/>
-    <col min="67" max="68" width="3.59765625" style="9" customWidth="1"/>
-    <col min="69" max="69" width="73.265625" style="9" customWidth="1"/>
-    <col min="70" max="70" width="2.59765625" style="9" customWidth="1"/>
-    <col min="71" max="16384" width="9" style="9"/>
+    <col min="8" max="8" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="15" max="18" width="3.578125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="3.578125" style="19" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="26" max="32" width="3.578125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="3.578125" style="19" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="3.578125" style="19" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="3.578125" style="9" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="5.3671875" style="9" customWidth="1"/>
+    <col min="39" max="41" width="3.578125" style="9" customWidth="1"/>
+    <col min="42" max="42" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="3.578125" style="131" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="46" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="3.578125" style="9" customWidth="1"/>
+    <col min="48" max="48" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="3.578125" style="105" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="60" max="60" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="3.578125" style="84" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="67" max="67" width="3.578125" style="19" customWidth="1"/>
+    <col min="68" max="69" width="3.578125" style="9" customWidth="1"/>
+    <col min="70" max="70" width="73.26171875" style="9" customWidth="1"/>
+    <col min="71" max="71" width="2.578125" style="9" customWidth="1"/>
+    <col min="72" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:70" outlineLevel="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:71" outlineLevel="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="5" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="37"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -5761,27 +5768,28 @@
       <c r="AM5" s="37"/>
       <c r="AN5" s="37"/>
       <c r="AO5" s="37"/>
-      <c r="AQ5" s="37"/>
+      <c r="AP5" s="37"/>
       <c r="AR5" s="37"/>
       <c r="AS5" s="37"/>
       <c r="AT5" s="37"/>
       <c r="AU5" s="37"/>
-      <c r="AW5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="BA5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BK5" s="37"/>
-      <c r="BM5" s="37"/>
+      <c r="AV5" s="37"/>
+      <c r="AX5" s="37"/>
+      <c r="AZ5" s="37"/>
+      <c r="BB5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BL5" s="37"/>
       <c r="BN5" s="37"/>
       <c r="BO5" s="37"/>
       <c r="BP5" s="37"/>
       <c r="BQ5" s="37"/>
       <c r="BR5" s="37"/>
+      <c r="BS5" s="37"/>
     </row>
-    <row r="6" spans="2:70" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:71" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4"/>
       <c r="C6" s="49" t="s">
         <v>0</v>
@@ -5822,37 +5830,38 @@
       <c r="AM6" s="11"/>
       <c r="AN6" s="11"/>
       <c r="AO6" s="11"/>
-      <c r="AP6" s="136"/>
-      <c r="AQ6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="132"/>
       <c r="AR6" s="11"/>
       <c r="AS6" s="11"/>
       <c r="AT6" s="11"/>
       <c r="AU6" s="11"/>
-      <c r="AV6" s="89"/>
-      <c r="AW6" s="11"/>
-      <c r="AX6" s="110"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="89"/>
-      <c r="BA6" s="11"/>
-      <c r="BB6" s="89"/>
-      <c r="BC6" s="11"/>
-      <c r="BD6" s="89"/>
-      <c r="BE6" s="11"/>
-      <c r="BF6" s="89"/>
-      <c r="BG6" s="11"/>
-      <c r="BH6" s="89"/>
-      <c r="BI6" s="11"/>
-      <c r="BJ6" s="89"/>
-      <c r="BK6" s="11"/>
-      <c r="BL6" s="89"/>
-      <c r="BM6" s="11"/>
-      <c r="BN6" s="10"/>
-      <c r="BO6" s="11"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="85"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="106"/>
+      <c r="AZ6" s="11"/>
+      <c r="BA6" s="85"/>
+      <c r="BB6" s="11"/>
+      <c r="BC6" s="85"/>
+      <c r="BD6" s="11"/>
+      <c r="BE6" s="85"/>
+      <c r="BF6" s="11"/>
+      <c r="BG6" s="85"/>
+      <c r="BH6" s="11"/>
+      <c r="BI6" s="85"/>
+      <c r="BJ6" s="11"/>
+      <c r="BK6" s="85"/>
+      <c r="BL6" s="11"/>
+      <c r="BM6" s="85"/>
+      <c r="BN6" s="11"/>
+      <c r="BO6" s="10"/>
       <c r="BP6" s="11"/>
       <c r="BQ6" s="11"/>
-      <c r="BR6" s="12"/>
+      <c r="BR6" s="11"/>
+      <c r="BS6" s="12"/>
     </row>
-    <row r="7" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4"/>
       <c r="C7" s="50"/>
       <c r="D7" s="50"/>
@@ -5893,209 +5902,213 @@
       <c r="AM7" s="14"/>
       <c r="AN7" s="14"/>
       <c r="AO7" s="14"/>
-      <c r="AP7" s="137"/>
-      <c r="AQ7" s="14"/>
+      <c r="AP7" s="14"/>
+      <c r="AQ7" s="133"/>
       <c r="AR7" s="14"/>
       <c r="AS7" s="14"/>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
-      <c r="AV7" s="90"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="111"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="90"/>
-      <c r="BA7" s="14"/>
-      <c r="BB7" s="90"/>
-      <c r="BC7" s="14"/>
-      <c r="BD7" s="90"/>
-      <c r="BE7" s="14"/>
-      <c r="BF7" s="90"/>
-      <c r="BG7" s="14"/>
-      <c r="BH7" s="90"/>
-      <c r="BI7" s="14"/>
-      <c r="BJ7" s="90"/>
-      <c r="BK7" s="14"/>
-      <c r="BL7" s="90"/>
-      <c r="BM7" s="14"/>
-      <c r="BN7" s="13"/>
-      <c r="BO7" s="14"/>
+      <c r="AV7" s="14"/>
+      <c r="AW7" s="86"/>
+      <c r="AX7" s="14"/>
+      <c r="AY7" s="107"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="86"/>
+      <c r="BB7" s="14"/>
+      <c r="BC7" s="86"/>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="86"/>
+      <c r="BF7" s="14"/>
+      <c r="BG7" s="86"/>
+      <c r="BH7" s="14"/>
+      <c r="BI7" s="86"/>
+      <c r="BJ7" s="14"/>
+      <c r="BK7" s="86"/>
+      <c r="BL7" s="14"/>
+      <c r="BM7" s="86"/>
+      <c r="BN7" s="14"/>
+      <c r="BO7" s="13"/>
       <c r="BP7" s="14"/>
       <c r="BQ7" s="14"/>
-      <c r="BR7" s="12"/>
+      <c r="BR7" s="14"/>
+      <c r="BS7" s="12"/>
     </row>
-    <row r="8" spans="2:70" s="103" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="93"/>
-      <c r="C8" s="94" t="s">
+    <row r="8" spans="2:71" s="99" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="89"/>
+      <c r="C8" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="97" t="s">
+      <c r="D8" s="90"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="93" t="s">
         <v>147</v>
       </c>
-      <c r="H8" s="98" t="s">
+      <c r="H8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="99" t="s">
+      <c r="I8" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="J8" s="98" t="s">
+      <c r="J8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="99" t="s">
+      <c r="K8" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="99" t="s">
+      <c r="L8" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="98" t="s">
+      <c r="M8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="99" t="s">
+      <c r="N8" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="99" t="s">
+      <c r="O8" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="P8" s="99" t="s">
+      <c r="P8" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="Q8" s="99" t="s">
+      <c r="Q8" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="R8" s="99" t="s">
+      <c r="R8" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="S8" s="98" t="s">
+      <c r="S8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="99" t="s">
+      <c r="T8" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="U8" s="98" t="s">
+      <c r="U8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="V8" s="99" t="s">
+      <c r="V8" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="W8" s="99" t="s">
+      <c r="W8" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="X8" s="98" t="s">
+      <c r="X8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="Y8" s="100" t="s">
+      <c r="Y8" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="Z8" s="99" t="s">
+      <c r="Z8" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="99" t="s">
+      <c r="AA8" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="AB8" s="99" t="s">
+      <c r="AB8" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="99" t="s">
+      <c r="AC8" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="AD8" s="99" t="s">
+      <c r="AD8" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="AE8" s="99" t="s">
+      <c r="AE8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="AF8" s="99" t="s">
+      <c r="AF8" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="AG8" s="98" t="s">
+      <c r="AG8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="AH8" s="101" t="s">
+      <c r="AH8" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="AI8" s="99"/>
-      <c r="AJ8" s="98" t="s">
+      <c r="AI8" s="95"/>
+      <c r="AJ8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="AK8" s="100" t="s">
+      <c r="AK8" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="AL8" s="100" t="s">
+      <c r="AL8" s="96" t="s">
         <v>211</v>
       </c>
-      <c r="AM8" s="100" t="s">
+      <c r="AM8" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="AN8" s="100" t="s">
+      <c r="AN8" s="96" t="s">
+        <v>210</v>
+      </c>
+      <c r="AO8" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="AO8" s="100" t="s">
+      <c r="AP8" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="AQ8" s="134" t="s">
         <v>209</v>
       </c>
-      <c r="AP8" s="138" t="s">
-        <v>210</v>
-      </c>
-      <c r="AQ8" s="100" t="str">
-        <f xml:space="preserve"> "count " &amp; AQ10</f>
+      <c r="AR8" s="96" t="str">
+        <f xml:space="preserve"> "count " &amp; AR10</f>
         <v>count ?</v>
       </c>
-      <c r="AR8" s="100" t="str">
-        <f t="shared" ref="AR8:AS8" si="0" xml:space="preserve"> "count " &amp; AR10</f>
+      <c r="AS8" s="96" t="str">
+        <f xml:space="preserve"> "count " &amp; AS10</f>
         <v>count A</v>
       </c>
-      <c r="AS8" s="100" t="str">
-        <f t="shared" si="0"/>
+      <c r="AT8" s="96" t="str">
+        <f xml:space="preserve"> "count " &amp; AT10</f>
         <v>count E</v>
       </c>
-      <c r="AT8" s="100"/>
-      <c r="AU8" s="99"/>
-      <c r="AV8" s="104" t="s">
+      <c r="AU8" s="96"/>
+      <c r="AV8" s="95"/>
+      <c r="AW8" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="AW8" s="99"/>
-      <c r="AX8" s="112" t="s">
+      <c r="AX8" s="95"/>
+      <c r="AY8" s="108" t="s">
         <v>174</v>
       </c>
-      <c r="AY8" s="99"/>
-      <c r="AZ8" s="104" t="s">
+      <c r="AZ8" s="95"/>
+      <c r="BA8" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="BA8" s="99"/>
-      <c r="BB8" s="104" t="s">
+      <c r="BB8" s="95"/>
+      <c r="BC8" s="100" t="s">
         <v>176</v>
       </c>
-      <c r="BC8" s="99"/>
-      <c r="BD8" s="104" t="s">
+      <c r="BD8" s="95"/>
+      <c r="BE8" s="100" t="s">
         <v>187</v>
       </c>
-      <c r="BE8" s="99"/>
-      <c r="BF8" s="104" t="s">
+      <c r="BF8" s="95"/>
+      <c r="BG8" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="BG8" s="99"/>
-      <c r="BH8" s="104" t="s">
+      <c r="BH8" s="95"/>
+      <c r="BI8" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="BI8" s="99"/>
-      <c r="BJ8" s="104" t="s">
+      <c r="BJ8" s="95"/>
+      <c r="BK8" s="100" t="s">
+        <v>206</v>
+      </c>
+      <c r="BL8" s="95"/>
+      <c r="BM8" s="100" t="s">
         <v>207</v>
       </c>
-      <c r="BK8" s="99"/>
-      <c r="BL8" s="104" t="s">
-        <v>208</v>
-      </c>
-      <c r="BM8" s="99"/>
-      <c r="BN8" s="98" t="s">
+      <c r="BN8" s="95"/>
+      <c r="BO8" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="BO8" s="99"/>
-      <c r="BP8" s="99"/>
+      <c r="BP8" s="95"/>
       <c r="BQ8" s="95"/>
-      <c r="BR8" s="102"/>
+      <c r="BR8" s="91"/>
+      <c r="BS8" s="98"/>
     </row>
-    <row r="9" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51"/>
@@ -6125,92 +6138,93 @@
       <c r="V9" s="42"/>
       <c r="W9" s="42"/>
       <c r="X9" s="42"/>
-      <c r="Y9" s="84"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="85"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="86"/>
+      <c r="Y9" s="140"/>
+      <c r="Z9" s="141"/>
+      <c r="AA9" s="141"/>
+      <c r="AB9" s="141"/>
+      <c r="AC9" s="141"/>
+      <c r="AD9" s="141"/>
+      <c r="AE9" s="141"/>
+      <c r="AF9" s="142"/>
       <c r="AG9" s="42"/>
       <c r="AH9" s="43"/>
       <c r="AI9" s="42"/>
       <c r="AJ9" s="42"/>
       <c r="AK9" s="76"/>
-      <c r="AL9" s="77"/>
-      <c r="AM9" s="77"/>
-      <c r="AN9" s="77"/>
+      <c r="AL9" s="82"/>
+      <c r="AM9" s="82"/>
+      <c r="AN9" s="82"/>
       <c r="AO9" s="77"/>
-      <c r="AP9" s="139"/>
-      <c r="AQ9" s="77"/>
+      <c r="AP9" s="77"/>
+      <c r="AQ9" s="135"/>
       <c r="AR9" s="77"/>
       <c r="AS9" s="77"/>
       <c r="AT9" s="77"/>
       <c r="AU9" s="77"/>
-      <c r="AV9" s="91" t="s">
+      <c r="AV9" s="77"/>
+      <c r="AW9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AW9" s="87" t="s">
+      <c r="AX9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="AX9" s="113" t="s">
+      <c r="AY9" s="109" t="s">
         <v>178</v>
       </c>
-      <c r="AY9" s="87" t="s">
+      <c r="AZ9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="AZ9" s="91" t="s">
+      <c r="BA9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BA9" s="87" t="s">
+      <c r="BB9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BB9" s="91" t="s">
+      <c r="BC9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BC9" s="87" t="s">
+      <c r="BD9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BD9" s="91" t="s">
+      <c r="BE9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BE9" s="87" t="s">
+      <c r="BF9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BF9" s="91" t="s">
+      <c r="BG9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BG9" s="87" t="s">
+      <c r="BH9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BH9" s="91" t="s">
+      <c r="BI9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BI9" s="87" t="s">
+      <c r="BJ9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BJ9" s="91" t="s">
+      <c r="BK9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BK9" s="87" t="s">
+      <c r="BL9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BL9" s="91" t="s">
+      <c r="BM9" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BM9" s="87" t="s">
+      <c r="BN9" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BN9" s="42"/>
       <c r="BO9" s="42"/>
       <c r="BP9" s="42"/>
-      <c r="BQ9" s="44" t="s">
+      <c r="BQ9" s="42"/>
+      <c r="BR9" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="BR9" s="12"/>
+      <c r="BS9" s="12"/>
     </row>
-    <row r="10" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="37"/>
       <c r="C10" s="52"/>
       <c r="D10" s="52"/>
@@ -6251,43 +6265,44 @@
       <c r="AM10" s="38"/>
       <c r="AN10" s="38"/>
       <c r="AO10" s="38"/>
-      <c r="AP10" s="140"/>
-      <c r="AQ10" s="38" t="s">
+      <c r="AP10" s="38"/>
+      <c r="AQ10" s="136"/>
+      <c r="AR10" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AR10" s="38" t="s">
+      <c r="AS10" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="AS10" s="38" t="s">
+      <c r="AT10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="AT10" s="38"/>
       <c r="AU10" s="38"/>
-      <c r="AV10" s="92"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="114"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="92"/>
-      <c r="BA10" s="38"/>
-      <c r="BB10" s="92"/>
-      <c r="BC10" s="38"/>
-      <c r="BD10" s="92"/>
-      <c r="BE10" s="38"/>
-      <c r="BF10" s="92"/>
-      <c r="BG10" s="38"/>
-      <c r="BH10" s="92"/>
-      <c r="BI10" s="38"/>
-      <c r="BJ10" s="92"/>
-      <c r="BK10" s="38"/>
-      <c r="BL10" s="92"/>
-      <c r="BM10" s="38"/>
+      <c r="AV10" s="38"/>
+      <c r="AW10" s="88"/>
+      <c r="AX10" s="38"/>
+      <c r="AY10" s="110"/>
+      <c r="AZ10" s="38"/>
+      <c r="BA10" s="88"/>
+      <c r="BB10" s="38"/>
+      <c r="BC10" s="88"/>
+      <c r="BD10" s="38"/>
+      <c r="BE10" s="88"/>
+      <c r="BF10" s="38"/>
+      <c r="BG10" s="88"/>
+      <c r="BH10" s="38"/>
+      <c r="BI10" s="88"/>
+      <c r="BJ10" s="38"/>
+      <c r="BK10" s="88"/>
+      <c r="BL10" s="38"/>
+      <c r="BM10" s="88"/>
       <c r="BN10" s="38"/>
       <c r="BO10" s="38"/>
       <c r="BP10" s="38"/>
       <c r="BQ10" s="38"/>
-      <c r="BR10" s="37"/>
+      <c r="BR10" s="38"/>
+      <c r="BS10" s="37"/>
     </row>
-    <row r="11" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="37"/>
       <c r="C11" s="52"/>
       <c r="D11" s="52"/>
@@ -6325,46 +6340,50 @@
       <c r="AJ11" s="38"/>
       <c r="AK11" s="38"/>
       <c r="AL11" s="38">
-        <f>SUM(AL13:AL20)</f>
-        <v>153</v>
+        <f>SUM(AL13:AL30)</f>
+        <v>121</v>
       </c>
       <c r="AM11" s="38">
-        <f>SUM(AM13:AM20)</f>
-        <v>137</v>
+        <f>SUM(AM13:AM30)</f>
+        <v>15</v>
       </c>
       <c r="AN11" s="38"/>
-      <c r="AO11" s="38"/>
-      <c r="AP11" s="140"/>
-      <c r="AQ11" s="38"/>
+      <c r="AO11" s="38">
+        <f>SUM(AO13:AO30)</f>
+        <v>14</v>
+      </c>
+      <c r="AP11" s="38"/>
+      <c r="AQ11" s="136"/>
       <c r="AR11" s="38"/>
       <c r="AS11" s="38"/>
       <c r="AT11" s="38"/>
       <c r="AU11" s="38"/>
-      <c r="AV11" s="92"/>
-      <c r="AW11" s="38"/>
-      <c r="AX11" s="114"/>
-      <c r="AY11" s="38"/>
-      <c r="AZ11" s="92"/>
-      <c r="BA11" s="38"/>
-      <c r="BB11" s="92"/>
-      <c r="BC11" s="38"/>
-      <c r="BD11" s="92"/>
-      <c r="BE11" s="38"/>
-      <c r="BF11" s="92"/>
-      <c r="BG11" s="38"/>
-      <c r="BH11" s="92"/>
-      <c r="BI11" s="38"/>
-      <c r="BJ11" s="92"/>
-      <c r="BK11" s="38"/>
-      <c r="BL11" s="92"/>
-      <c r="BM11" s="38"/>
+      <c r="AV11" s="38"/>
+      <c r="AW11" s="88"/>
+      <c r="AX11" s="38"/>
+      <c r="AY11" s="110"/>
+      <c r="AZ11" s="38"/>
+      <c r="BA11" s="88"/>
+      <c r="BB11" s="38"/>
+      <c r="BC11" s="88"/>
+      <c r="BD11" s="38"/>
+      <c r="BE11" s="88"/>
+      <c r="BF11" s="38"/>
+      <c r="BG11" s="88"/>
+      <c r="BH11" s="38"/>
+      <c r="BI11" s="88"/>
+      <c r="BJ11" s="38"/>
+      <c r="BK11" s="88"/>
+      <c r="BL11" s="38"/>
+      <c r="BM11" s="88"/>
       <c r="BN11" s="38"/>
       <c r="BO11" s="38"/>
       <c r="BP11" s="38"/>
       <c r="BQ11" s="38"/>
-      <c r="BR11" s="37"/>
+      <c r="BR11" s="38"/>
+      <c r="BS11" s="37"/>
     </row>
-    <row r="12" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="37"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
@@ -6405,47 +6424,48 @@
       <c r="AM12" s="38"/>
       <c r="AN12" s="38"/>
       <c r="AO12" s="38"/>
-      <c r="AP12" s="140"/>
-      <c r="AQ12" s="38"/>
+      <c r="AP12" s="38"/>
+      <c r="AQ12" s="136"/>
       <c r="AR12" s="38"/>
       <c r="AS12" s="38"/>
       <c r="AT12" s="38"/>
       <c r="AU12" s="38"/>
-      <c r="AV12" s="92"/>
-      <c r="AW12" s="38"/>
-      <c r="AX12" s="114"/>
-      <c r="AY12" s="38"/>
-      <c r="AZ12" s="92"/>
-      <c r="BA12" s="38"/>
-      <c r="BB12" s="92"/>
-      <c r="BC12" s="38"/>
-      <c r="BD12" s="92"/>
-      <c r="BE12" s="38"/>
-      <c r="BF12" s="92"/>
-      <c r="BG12" s="38"/>
-      <c r="BH12" s="92"/>
-      <c r="BI12" s="38"/>
-      <c r="BJ12" s="92"/>
-      <c r="BK12" s="38"/>
-      <c r="BL12" s="92"/>
-      <c r="BM12" s="38"/>
+      <c r="AV12" s="38"/>
+      <c r="AW12" s="88"/>
+      <c r="AX12" s="38"/>
+      <c r="AY12" s="110"/>
+      <c r="AZ12" s="38"/>
+      <c r="BA12" s="88"/>
+      <c r="BB12" s="38"/>
+      <c r="BC12" s="88"/>
+      <c r="BD12" s="38"/>
+      <c r="BE12" s="88"/>
+      <c r="BF12" s="38"/>
+      <c r="BG12" s="88"/>
+      <c r="BH12" s="38"/>
+      <c r="BI12" s="88"/>
+      <c r="BJ12" s="38"/>
+      <c r="BK12" s="88"/>
+      <c r="BL12" s="38"/>
+      <c r="BM12" s="88"/>
       <c r="BN12" s="38"/>
       <c r="BO12" s="38"/>
       <c r="BP12" s="38"/>
       <c r="BQ12" s="38"/>
-      <c r="BR12" s="37"/>
+      <c r="BR12" s="38"/>
+      <c r="BS12" s="37"/>
     </row>
-    <row r="13" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:71" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4"/>
       <c r="C13" s="18"/>
       <c r="D13" s="53"/>
-      <c r="E13" s="105" t="s">
+      <c r="E13" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="107" t="s">
+      <c r="G13" s="103" t="s">
         <v>148</v>
       </c>
       <c r="H13" s="16"/>
@@ -6489,111 +6509,114 @@
       <c r="AJ13" s="16"/>
       <c r="AK13" s="7"/>
       <c r="AL13" s="7">
-        <f>AN13*AO13:AO14</f>
+        <f>AM13*AS13</f>
         <v>32</v>
       </c>
       <c r="AM13" s="7">
-        <f>AN13*AP13</f>
+        <f>AN13*AO13</f>
+        <v>2</v>
+      </c>
+      <c r="AN13" s="7">
+        <v>2</v>
+      </c>
+      <c r="AO13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="7">
+        <f>SUM(AR13:AT13)</f>
         <v>32</v>
       </c>
-      <c r="AN13" s="7">
-        <v>1</v>
-      </c>
-      <c r="AO13" s="7">
-        <f>SUM(AQ13:AS13)</f>
+      <c r="AQ13" s="136">
+        <f>SUM(AS13:AT13)</f>
         <v>32</v>
       </c>
-      <c r="AP13" s="140">
-        <f>SUM(AR13:AS13)</f>
-        <v>32</v>
-      </c>
-      <c r="AQ13" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV13:$BM13)))))</f>
+      <c r="AR13" s="7">
+        <f t="shared" ref="AR13:AT20" si="0">SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AW13:$BN13)))))</f>
         <v>0</v>
       </c>
-      <c r="AR13" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV13:$BM13)))))</f>
+      <c r="AS13" s="7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AS13" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV13:$BM13)))))</f>
+      <c r="AT13" s="7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AT13" s="7"/>
       <c r="AU13" s="7"/>
-      <c r="AV13" s="92" t="s">
+      <c r="AV13" s="7"/>
+      <c r="AW13" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="AW13" s="7" t="s">
+      <c r="AX13" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AX13" s="115" t="s">
+      <c r="AY13" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="AY13" s="40" t="s">
+      <c r="AZ13" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="AZ13" s="92" t="s">
+      <c r="BA13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BA13" s="7" t="s">
+      <c r="BB13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BB13" s="92" t="s">
+      <c r="BC13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BC13" s="7" t="s">
+      <c r="BD13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BD13" s="92" t="s">
+      <c r="BE13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BE13" s="7" t="s">
+      <c r="BF13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BF13" s="92" t="s">
+      <c r="BG13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BG13" s="7" t="s">
+      <c r="BH13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BH13" s="92" t="s">
+      <c r="BI13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BI13" s="7" t="s">
+      <c r="BJ13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BJ13" s="92" t="s">
+      <c r="BK13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BK13" s="7" t="s">
+      <c r="BL13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BL13" s="92" t="s">
+      <c r="BM13" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BM13" s="7" t="s">
+      <c r="BN13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BN13" s="16"/>
-      <c r="BO13" s="7"/>
+      <c r="BO13" s="16"/>
       <c r="BP13" s="7"/>
-      <c r="BQ13" s="17" t="s">
+      <c r="BQ13" s="7"/>
+      <c r="BR13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BR13" s="12"/>
+      <c r="BS13" s="12"/>
     </row>
-    <row r="14" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:71" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4"/>
       <c r="C14" s="18"/>
       <c r="D14" s="53"/>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="106" t="s">
+      <c r="F14" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="107" t="s">
+      <c r="G14" s="103" t="s">
         <v>148</v>
       </c>
       <c r="H14" s="16"/>
@@ -6633,111 +6656,114 @@
       <c r="AJ14" s="16"/>
       <c r="AK14" s="7"/>
       <c r="AL14" s="7">
-        <f t="shared" ref="AL14:AL20" si="1">AN14*AO14:AO15</f>
-        <v>64</v>
+        <f t="shared" ref="AL14:AL20" si="1">AN14*AO14*AS14</f>
+        <v>32</v>
       </c>
       <c r="AM14" s="7">
-        <f t="shared" ref="AM14:AM20" si="2">AN14*AP14</f>
-        <v>64</v>
+        <f t="shared" ref="AM14:AM20" si="2">AN14*AO14</f>
+        <v>2</v>
       </c>
       <c r="AN14" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="7">
         <v>2</v>
       </c>
-      <c r="AO14" s="7">
-        <f t="shared" ref="AO14:AO20" si="3">SUM(AQ14:AS14)</f>
+      <c r="AP14" s="7">
+        <f t="shared" ref="AP14:AP20" si="3">SUM(AR14:AT14)</f>
         <v>32</v>
       </c>
-      <c r="AP14" s="140">
-        <f t="shared" ref="AP14:AP20" si="4">SUM(AR14:AS14)</f>
+      <c r="AQ14" s="136">
+        <f t="shared" ref="AQ14:AQ20" si="4">SUM(AS14:AT14)</f>
         <v>32</v>
       </c>
-      <c r="AQ14" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV14:$BM14)))))</f>
+      <c r="AR14" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR14" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV14:$BM14)))))</f>
+      <c r="AS14" s="7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AS14" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV14:$BM14)))))</f>
+      <c r="AT14" s="7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AT14" s="7"/>
       <c r="AU14" s="7"/>
-      <c r="AV14" s="92" t="s">
+      <c r="AV14" s="7"/>
+      <c r="AW14" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="AW14" s="7" t="s">
+      <c r="AX14" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AX14" s="115" t="s">
+      <c r="AY14" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="AY14" s="40" t="s">
+      <c r="AZ14" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="AZ14" s="92" t="s">
+      <c r="BA14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BA14" s="7" t="s">
+      <c r="BB14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BB14" s="92" t="s">
+      <c r="BC14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BC14" s="7" t="s">
+      <c r="BD14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BD14" s="92" t="s">
+      <c r="BE14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BE14" s="7" t="s">
+      <c r="BF14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BF14" s="92" t="s">
+      <c r="BG14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BG14" s="7" t="s">
+      <c r="BH14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BH14" s="92" t="s">
+      <c r="BI14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BI14" s="7" t="s">
+      <c r="BJ14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BJ14" s="92" t="s">
+      <c r="BK14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BK14" s="7" t="s">
+      <c r="BL14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BL14" s="92" t="s">
+      <c r="BM14" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BM14" s="7" t="s">
+      <c r="BN14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BN14" s="16"/>
-      <c r="BO14" s="7"/>
+      <c r="BO14" s="16"/>
       <c r="BP14" s="7"/>
-      <c r="BQ14" s="18" t="s">
+      <c r="BQ14" s="7"/>
+      <c r="BR14" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="BR14" s="12"/>
+      <c r="BS14" s="12"/>
     </row>
-    <row r="15" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:71" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4"/>
       <c r="C15" s="18"/>
       <c r="D15" s="53"/>
-      <c r="E15" s="108" t="s">
+      <c r="E15" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="106" t="s">
+      <c r="F15" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="107" t="s">
+      <c r="G15" s="103" t="s">
         <v>148</v>
       </c>
       <c r="H15" s="16"/>
@@ -6778,110 +6804,113 @@
       <c r="AK15" s="7"/>
       <c r="AL15" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AM15" s="7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO15" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="7">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="AP15" s="140">
+      <c r="AQ15" s="136">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="AQ15" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV15:$BM15)))))</f>
+      <c r="AR15" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR15" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV15:$BM15)))))</f>
+      <c r="AS15" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AS15" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV15:$BM15)))))</f>
+      <c r="AT15" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AT15" s="7"/>
       <c r="AU15" s="7"/>
-      <c r="AV15" s="92" t="s">
+      <c r="AV15" s="7"/>
+      <c r="AW15" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="AW15" s="7" t="s">
+      <c r="AX15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AX15" s="114" t="s">
+      <c r="AY15" s="110" t="s">
         <v>177</v>
       </c>
-      <c r="AY15" s="7" t="s">
+      <c r="AZ15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AZ15" s="92" t="s">
+      <c r="BA15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BA15" s="7" t="s">
+      <c r="BB15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BB15" s="92" t="s">
+      <c r="BC15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BC15" s="7" t="s">
+      <c r="BD15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BD15" s="92" t="s">
+      <c r="BE15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BE15" s="7" t="s">
+      <c r="BF15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BF15" s="92" t="s">
+      <c r="BG15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BG15" s="7" t="s">
+      <c r="BH15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BH15" s="92" t="s">
+      <c r="BI15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BI15" s="7" t="s">
+      <c r="BJ15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BJ15" s="92" t="s">
+      <c r="BK15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BK15" s="7" t="s">
+      <c r="BL15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BL15" s="92" t="s">
+      <c r="BM15" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="BM15" s="7" t="s">
+      <c r="BN15" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BN15" s="16"/>
-      <c r="BO15" s="7"/>
+      <c r="BO15" s="16"/>
       <c r="BP15" s="7"/>
-      <c r="BQ15" s="18" t="s">
+      <c r="BQ15" s="7"/>
+      <c r="BR15" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="BR15" s="12"/>
+      <c r="BS15" s="12"/>
     </row>
-    <row r="16" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:71" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4"/>
       <c r="C16" s="18"/>
       <c r="D16" s="53"/>
-      <c r="E16" s="108" t="s">
+      <c r="E16" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="106" t="s">
+      <c r="F16" s="102" t="s">
         <v>186</v>
       </c>
-      <c r="G16" s="107" t="s">
+      <c r="G16" s="103" t="s">
         <v>148</v>
       </c>
       <c r="H16" s="16"/>
@@ -6922,110 +6951,113 @@
       <c r="AK16" s="7"/>
       <c r="AL16" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="AM16" s="7">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="AN16" s="7">
         <v>1</v>
       </c>
       <c r="AO16" s="7">
+        <v>2</v>
+      </c>
+      <c r="AP16" s="7">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="AP16" s="140">
+      <c r="AQ16" s="136">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="AQ16" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV16:$BM16)))))</f>
+      <c r="AR16" s="7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AR16" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV16:$BM16)))))</f>
+      <c r="AS16" s="7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AS16" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV16:$BM16)))))</f>
+      <c r="AT16" s="7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AT16" s="7"/>
       <c r="AU16" s="7"/>
-      <c r="AV16" s="92" t="s">
+      <c r="AV16" s="7"/>
+      <c r="AW16" s="88" t="s">
         <v>177</v>
       </c>
-      <c r="AW16" s="7" t="s">
+      <c r="AX16" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AX16" s="115" t="s">
+      <c r="AY16" s="111" t="s">
         <v>177</v>
       </c>
-      <c r="AY16" s="40" t="s">
+      <c r="AZ16" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="AZ16" s="92" t="s">
+      <c r="BA16" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BA16" s="7" t="s">
+      <c r="BB16" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BB16" s="92" t="s">
+      <c r="BC16" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BC16" s="7" t="s">
+      <c r="BD16" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BD16" s="92" t="s">
+      <c r="BE16" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BE16" s="7" t="s">
+      <c r="BF16" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BF16" s="116" t="s">
+      <c r="BG16" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="BG16" s="40" t="s">
+      <c r="BH16" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="BH16" s="92" t="s">
+      <c r="BI16" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BI16" s="7" t="s">
+      <c r="BJ16" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BJ16" s="92" t="s">
+      <c r="BK16" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BK16" s="7" t="s">
+      <c r="BL16" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BL16" s="92" t="s">
+      <c r="BM16" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BM16" s="7" t="s">
+      <c r="BN16" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BN16" s="16"/>
-      <c r="BO16" s="7"/>
+      <c r="BO16" s="16"/>
       <c r="BP16" s="7"/>
-      <c r="BQ16" s="18" t="s">
+      <c r="BQ16" s="7"/>
+      <c r="BR16" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="BR16" s="12"/>
+      <c r="BS16" s="12"/>
     </row>
-    <row r="17" spans="2:70" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:71" ht="31.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4"/>
       <c r="C17" s="18"/>
       <c r="D17" s="53"/>
-      <c r="E17" s="105" t="s">
+      <c r="E17" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="107" t="s">
+      <c r="F17" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="G17" s="107" t="s">
+      <c r="G17" s="103" t="s">
         <v>148</v>
       </c>
       <c r="H17" s="16"/>
@@ -7082,88 +7114,91 @@
       <c r="AK17" s="7"/>
       <c r="AL17" s="7">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="AM17" s="7">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AN17" s="7">
         <v>1</v>
       </c>
       <c r="AO17" s="7">
+        <v>2</v>
+      </c>
+      <c r="AP17" s="7">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="AP17" s="140">
+      <c r="AQ17" s="136">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AQ17" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV17:$BM17)))))</f>
+      <c r="AR17" s="7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AR17" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV17:$BM17)))))</f>
+      <c r="AS17" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AS17" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV17:$BM17)))))</f>
+      <c r="AT17" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AT17" s="7"/>
       <c r="AU17" s="7"/>
-      <c r="AV17" s="92"/>
-      <c r="AW17" s="7"/>
-      <c r="AX17" s="114"/>
-      <c r="AY17" s="7"/>
-      <c r="AZ17" s="92"/>
-      <c r="BA17" s="7"/>
-      <c r="BB17" s="92" t="s">
+      <c r="AV17" s="7"/>
+      <c r="AW17" s="88"/>
+      <c r="AX17" s="7"/>
+      <c r="AY17" s="110"/>
+      <c r="AZ17" s="7"/>
+      <c r="BA17" s="88"/>
+      <c r="BB17" s="7"/>
+      <c r="BC17" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BC17" s="7" t="s">
+      <c r="BD17" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BD17" s="92" t="s">
+      <c r="BE17" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="BE17" s="7" t="s">
+      <c r="BF17" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="BF17" s="92" t="s">
+      <c r="BG17" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BG17" s="7" t="s">
+      <c r="BH17" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BH17" s="92" t="s">
+      <c r="BI17" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BI17" s="7" t="s">
+      <c r="BJ17" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BJ17" s="92" t="s">
+      <c r="BK17" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BK17" s="7" t="s">
+      <c r="BL17" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BL17" s="92" t="s">
+      <c r="BM17" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BM17" s="7" t="s">
+      <c r="BN17" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BN17" s="16"/>
-      <c r="BO17" s="7"/>
+      <c r="BO17" s="16"/>
       <c r="BP17" s="7"/>
-      <c r="BQ17" s="18" t="s">
+      <c r="BQ17" s="7"/>
+      <c r="BR17" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="BR17" s="12"/>
+      <c r="BS17" s="12"/>
     </row>
-    <row r="18" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:71" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="4"/>
       <c r="C18" s="18"/>
       <c r="D18" s="53"/>
@@ -7244,80 +7279,83 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN18" s="7"/>
-      <c r="AO18" s="7">
+      <c r="AN18" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="7">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="AP18" s="140">
+      <c r="AQ18" s="136">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AQ18" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV18:$BM18)))))</f>
+      <c r="AR18" s="7">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AR18" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV18:$BM18)))))</f>
+      <c r="AS18" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS18" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV18:$BM18)))))</f>
+      <c r="AT18" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AT18" s="7"/>
       <c r="AU18" s="7"/>
-      <c r="AV18" s="92"/>
-      <c r="AW18" s="7"/>
-      <c r="AX18" s="114"/>
-      <c r="AY18" s="7"/>
-      <c r="AZ18" s="92"/>
-      <c r="BA18" s="7"/>
-      <c r="BB18" s="92" t="s">
+      <c r="AV18" s="7"/>
+      <c r="AW18" s="88"/>
+      <c r="AX18" s="7"/>
+      <c r="AY18" s="110"/>
+      <c r="AZ18" s="7"/>
+      <c r="BA18" s="88"/>
+      <c r="BB18" s="7"/>
+      <c r="BC18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BC18" s="7" t="s">
+      <c r="BD18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BD18" s="92" t="s">
+      <c r="BE18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BE18" s="7" t="s">
+      <c r="BF18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BF18" s="92" t="s">
+      <c r="BG18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BG18" s="7" t="s">
+      <c r="BH18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BH18" s="92" t="s">
+      <c r="BI18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BI18" s="7" t="s">
+      <c r="BJ18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BJ18" s="92" t="s">
+      <c r="BK18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BK18" s="7" t="s">
+      <c r="BL18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BL18" s="92" t="s">
+      <c r="BM18" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BM18" s="7" t="s">
+      <c r="BN18" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BN18" s="16"/>
-      <c r="BO18" s="7"/>
+      <c r="BO18" s="16"/>
       <c r="BP18" s="7"/>
-      <c r="BQ18" s="18" t="s">
+      <c r="BQ18" s="7"/>
+      <c r="BR18" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="BR18" s="8"/>
+      <c r="BS18" s="8"/>
     </row>
-    <row r="19" spans="2:70" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:71" ht="15.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4"/>
       <c r="C19" s="18"/>
       <c r="D19" s="53"/>
@@ -7398,80 +7436,83 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN19" s="7"/>
-      <c r="AO19" s="7">
+      <c r="AN19" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="7"/>
+      <c r="AP19" s="7">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="AP19" s="140">
+      <c r="AQ19" s="136">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AQ19" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV19:$BM19)))))</f>
+      <c r="AR19" s="7">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AR19" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV19:$BM19)))))</f>
+      <c r="AS19" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS19" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV19:$BM19)))))</f>
+      <c r="AT19" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AT19" s="7"/>
       <c r="AU19" s="7"/>
-      <c r="AV19" s="92"/>
-      <c r="AW19" s="7"/>
-      <c r="AX19" s="114"/>
-      <c r="AY19" s="7"/>
-      <c r="AZ19" s="92"/>
-      <c r="BA19" s="7"/>
-      <c r="BB19" s="92" t="s">
+      <c r="AV19" s="7"/>
+      <c r="AW19" s="88"/>
+      <c r="AX19" s="7"/>
+      <c r="AY19" s="110"/>
+      <c r="AZ19" s="7"/>
+      <c r="BA19" s="88"/>
+      <c r="BB19" s="7"/>
+      <c r="BC19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BC19" s="7" t="s">
+      <c r="BD19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BD19" s="92" t="s">
+      <c r="BE19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BE19" s="7" t="s">
+      <c r="BF19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BF19" s="92" t="s">
+      <c r="BG19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BG19" s="7" t="s">
+      <c r="BH19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BH19" s="92" t="s">
+      <c r="BI19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BI19" s="7" t="s">
+      <c r="BJ19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BJ19" s="92" t="s">
+      <c r="BK19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BK19" s="7" t="s">
+      <c r="BL19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BL19" s="92" t="s">
+      <c r="BM19" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="BM19" s="7" t="s">
+      <c r="BN19" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="BN19" s="16"/>
-      <c r="BO19" s="7"/>
+      <c r="BO19" s="16"/>
       <c r="BP19" s="7"/>
-      <c r="BQ19" s="18" t="s">
+      <c r="BQ19" s="7"/>
+      <c r="BR19" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="BR19" s="8"/>
+      <c r="BS19" s="8"/>
     </row>
-    <row r="20" spans="2:70" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:71" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4"/>
       <c r="C20" s="18"/>
       <c r="D20" s="53"/>
@@ -7524,92 +7565,95 @@
       </c>
       <c r="AM20" s="7">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="AN20" s="7">
         <v>1</v>
       </c>
       <c r="AO20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="7">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="AP20" s="140">
+      <c r="AQ20" s="136">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="AQ20" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AQ$10,UPPER($AV20:$BM20)))))</f>
+      <c r="AR20" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR20" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AR$10,UPPER($AV20:$BM20)))))</f>
+      <c r="AS20" s="7">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="AS20" s="7">
-        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AV20:$BM20)))))</f>
+      <c r="AT20" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AT20" s="7"/>
       <c r="AU20" s="7"/>
-      <c r="AV20" s="92" t="s">
+      <c r="AV20" s="7"/>
+      <c r="AW20" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AW20" s="7"/>
-      <c r="AX20" s="114" t="s">
+      <c r="AX20" s="7"/>
+      <c r="AY20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="AY20" s="7" t="s">
+      <c r="AZ20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="AZ20" s="114" t="s">
+      <c r="BA20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BA20" s="7" t="s">
+      <c r="BB20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BB20" s="114" t="s">
+      <c r="BC20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BC20" s="7" t="s">
+      <c r="BD20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BD20" s="114" t="s">
+      <c r="BE20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BE20" s="7" t="s">
+      <c r="BF20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BF20" s="114" t="s">
+      <c r="BG20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BG20" s="7" t="s">
+      <c r="BH20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BH20" s="114" t="s">
+      <c r="BI20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BI20" s="7" t="s">
+      <c r="BJ20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BJ20" s="114" t="s">
+      <c r="BK20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BK20" s="7" t="s">
+      <c r="BL20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BL20" s="114" t="s">
+      <c r="BM20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="BM20" s="7" t="s">
+      <c r="BN20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="BN20" s="16"/>
-      <c r="BO20" s="7"/>
+      <c r="BO20" s="16"/>
       <c r="BP20" s="7"/>
-      <c r="BQ20" s="18"/>
-      <c r="BR20" s="12"/>
+      <c r="BQ20" s="7"/>
+      <c r="BR20" s="18"/>
+      <c r="BS20" s="12"/>
     </row>
-    <row r="21" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="37"/>
       <c r="C21" s="52"/>
       <c r="D21" s="52"/>
@@ -7650,299 +7694,300 @@
       <c r="AM21" s="38"/>
       <c r="AN21" s="38"/>
       <c r="AO21" s="38"/>
-      <c r="AP21" s="140"/>
-      <c r="AQ21" s="38"/>
+      <c r="AP21" s="38"/>
+      <c r="AQ21" s="136"/>
       <c r="AR21" s="38"/>
       <c r="AS21" s="38"/>
       <c r="AT21" s="38"/>
       <c r="AU21" s="38"/>
-      <c r="AV21" s="92"/>
-      <c r="AW21" s="38"/>
-      <c r="AX21" s="114"/>
-      <c r="AY21" s="38"/>
-      <c r="AZ21" s="92"/>
-      <c r="BA21" s="38"/>
-      <c r="BB21" s="92"/>
-      <c r="BC21" s="38"/>
-      <c r="BD21" s="92"/>
-      <c r="BE21" s="38"/>
-      <c r="BF21" s="92"/>
-      <c r="BG21" s="38"/>
-      <c r="BH21" s="92"/>
-      <c r="BI21" s="38"/>
-      <c r="BJ21" s="92"/>
-      <c r="BK21" s="38"/>
-      <c r="BL21" s="92"/>
-      <c r="BM21" s="38"/>
+      <c r="AV21" s="38"/>
+      <c r="AW21" s="88"/>
+      <c r="AX21" s="38"/>
+      <c r="AY21" s="110"/>
+      <c r="AZ21" s="38"/>
+      <c r="BA21" s="88"/>
+      <c r="BB21" s="38"/>
+      <c r="BC21" s="88"/>
+      <c r="BD21" s="38"/>
+      <c r="BE21" s="88"/>
+      <c r="BF21" s="38"/>
+      <c r="BG21" s="88"/>
+      <c r="BH21" s="38"/>
+      <c r="BI21" s="88"/>
+      <c r="BJ21" s="38"/>
+      <c r="BK21" s="88"/>
+      <c r="BL21" s="38"/>
+      <c r="BM21" s="88"/>
       <c r="BN21" s="38"/>
       <c r="BO21" s="38"/>
       <c r="BP21" s="38"/>
       <c r="BQ21" s="38"/>
-      <c r="BR21" s="37"/>
+      <c r="BR21" s="38"/>
+      <c r="BS21" s="37"/>
     </row>
-    <row r="22" spans="2:70" s="103" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="93"/>
-      <c r="C22" s="94" t="s">
+    <row r="22" spans="2:71" s="99" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="89"/>
+      <c r="C22" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="94"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="97" t="s">
+      <c r="D22" s="90"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="93" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I22" s="99" t="s">
+      <c r="I22" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="J22" s="98" t="s">
+      <c r="J22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="99" t="s">
+      <c r="K22" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="L22" s="99" t="s">
+      <c r="L22" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="M22" s="98" t="s">
+      <c r="M22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="99" t="s">
+      <c r="N22" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="O22" s="99" t="s">
+      <c r="O22" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="P22" s="99" t="s">
+      <c r="P22" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="Q22" s="99" t="s">
+      <c r="Q22" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="R22" s="99" t="s">
+      <c r="R22" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="S22" s="98" t="s">
+      <c r="S22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="T22" s="99" t="s">
+      <c r="T22" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="U22" s="98" t="s">
+      <c r="U22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="V22" s="99" t="s">
+      <c r="V22" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="W22" s="99" t="s">
+      <c r="W22" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="X22" s="98" t="s">
+      <c r="X22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="Y22" s="100" t="s">
+      <c r="Y22" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="Z22" s="99" t="s">
+      <c r="Z22" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="AA22" s="99" t="s">
+      <c r="AA22" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="AB22" s="99" t="s">
+      <c r="AB22" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="AC22" s="99" t="s">
+      <c r="AC22" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="AD22" s="99" t="s">
+      <c r="AD22" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="AE22" s="99" t="s">
+      <c r="AE22" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="AF22" s="99" t="s">
+      <c r="AF22" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="AG22" s="98" t="s">
+      <c r="AG22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="AH22" s="101" t="s">
+      <c r="AH22" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="AI22" s="99"/>
-      <c r="AJ22" s="98" t="s">
+      <c r="AI22" s="95"/>
+      <c r="AJ22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="AK22" s="100" t="s">
+      <c r="AK22" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="AL22" s="100"/>
-      <c r="AM22" s="100" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN22" s="100"/>
-      <c r="AO22" s="100"/>
-      <c r="AP22" s="138"/>
-      <c r="AQ22" s="100"/>
-      <c r="AR22" s="100"/>
-      <c r="AS22" s="100"/>
-      <c r="AT22" s="100"/>
-      <c r="AU22" s="99"/>
-      <c r="AV22" s="104" t="s">
+      <c r="AL22" s="96"/>
+      <c r="AM22" s="96"/>
+      <c r="AN22" s="96"/>
+      <c r="AO22" s="96"/>
+      <c r="AP22" s="96"/>
+      <c r="AQ22" s="134"/>
+      <c r="AR22" s="96"/>
+      <c r="AS22" s="96"/>
+      <c r="AT22" s="96"/>
+      <c r="AU22" s="96"/>
+      <c r="AV22" s="95"/>
+      <c r="AW22" s="100" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX22" s="95"/>
+      <c r="AY22" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="AW22" s="99"/>
-      <c r="AX22" s="112" t="s">
+      <c r="AZ22" s="95"/>
+      <c r="BA22" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="AY22" s="99"/>
-      <c r="AZ22" s="104" t="s">
+      <c r="BB22" s="95"/>
+      <c r="BC22" s="100" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD22" s="95"/>
+      <c r="BE22" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="BF22" s="95"/>
+      <c r="BG22" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH22" s="95"/>
+      <c r="BI22" s="100"/>
+      <c r="BJ22" s="95"/>
+      <c r="BK22" s="100" t="s">
         <v>200</v>
       </c>
-      <c r="BA22" s="99"/>
-      <c r="BB22" s="104" t="s">
-        <v>202</v>
-      </c>
-      <c r="BC22" s="99"/>
-      <c r="BD22" s="104" t="s">
-        <v>203</v>
-      </c>
-      <c r="BE22" s="99"/>
-      <c r="BF22" s="104" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG22" s="99"/>
-      <c r="BH22" s="104"/>
-      <c r="BI22" s="99"/>
-      <c r="BJ22" s="104" t="s">
-        <v>201</v>
-      </c>
-      <c r="BK22" s="99"/>
-      <c r="BL22" s="104" t="s">
-        <v>201</v>
-      </c>
-      <c r="BM22" s="99"/>
-      <c r="BN22" s="98" t="s">
+      <c r="BL22" s="95"/>
+      <c r="BM22" s="100" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN22" s="95"/>
+      <c r="BO22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="BO22" s="99"/>
-      <c r="BP22" s="99"/>
+      <c r="BP22" s="95"/>
       <c r="BQ22" s="95"/>
-      <c r="BR22" s="102"/>
+      <c r="BR22" s="91"/>
+      <c r="BS22" s="98"/>
     </row>
-    <row r="23" spans="2:70" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:71" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="37"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="117"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="117"/>
-      <c r="J23" s="117"/>
-      <c r="K23" s="117"/>
-      <c r="L23" s="117"/>
-      <c r="M23" s="117"/>
-      <c r="N23" s="117"/>
-      <c r="O23" s="117"/>
-      <c r="P23" s="117"/>
-      <c r="Q23" s="117"/>
-      <c r="R23" s="117"/>
-      <c r="S23" s="117"/>
-      <c r="T23" s="117"/>
-      <c r="U23" s="117"/>
-      <c r="V23" s="117"/>
-      <c r="W23" s="117"/>
-      <c r="X23" s="117"/>
-      <c r="Y23" s="117"/>
-      <c r="Z23" s="117"/>
-      <c r="AA23" s="117"/>
-      <c r="AB23" s="117"/>
-      <c r="AC23" s="117"/>
-      <c r="AD23" s="117"/>
-      <c r="AE23" s="117"/>
-      <c r="AF23" s="117"/>
-      <c r="AG23" s="117"/>
-      <c r="AH23" s="117"/>
-      <c r="AI23" s="117"/>
-      <c r="AJ23" s="117"/>
-      <c r="AK23" s="117"/>
-      <c r="AL23" s="117"/>
-      <c r="AM23" s="117"/>
-      <c r="AN23" s="117"/>
-      <c r="AO23" s="117"/>
-      <c r="AP23" s="141"/>
-      <c r="AQ23" s="117"/>
-      <c r="AR23" s="117"/>
-      <c r="AS23" s="117"/>
-      <c r="AT23" s="117"/>
-      <c r="AU23" s="117"/>
-      <c r="AV23" s="91" t="s">
+      <c r="C23" s="114"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="113"/>
+      <c r="Q23" s="113"/>
+      <c r="R23" s="113"/>
+      <c r="S23" s="113"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="113"/>
+      <c r="V23" s="113"/>
+      <c r="W23" s="113"/>
+      <c r="X23" s="113"/>
+      <c r="Y23" s="113"/>
+      <c r="Z23" s="113"/>
+      <c r="AA23" s="113"/>
+      <c r="AB23" s="113"/>
+      <c r="AC23" s="113"/>
+      <c r="AD23" s="113"/>
+      <c r="AE23" s="113"/>
+      <c r="AF23" s="113"/>
+      <c r="AG23" s="113"/>
+      <c r="AH23" s="113"/>
+      <c r="AI23" s="113"/>
+      <c r="AJ23" s="113"/>
+      <c r="AK23" s="113"/>
+      <c r="AL23" s="113"/>
+      <c r="AM23" s="113"/>
+      <c r="AN23" s="113"/>
+      <c r="AO23" s="113"/>
+      <c r="AP23" s="113"/>
+      <c r="AQ23" s="137"/>
+      <c r="AR23" s="113"/>
+      <c r="AS23" s="113"/>
+      <c r="AT23" s="113"/>
+      <c r="AU23" s="113"/>
+      <c r="AV23" s="113"/>
+      <c r="AW23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AW23" s="87" t="s">
+      <c r="AX23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="AX23" s="113" t="s">
+      <c r="AY23" s="109" t="s">
         <v>178</v>
       </c>
-      <c r="AY23" s="87" t="s">
+      <c r="AZ23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="AZ23" s="91" t="s">
+      <c r="BA23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BA23" s="87" t="s">
+      <c r="BB23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BB23" s="91" t="s">
+      <c r="BC23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BC23" s="87" t="s">
+      <c r="BD23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BD23" s="91" t="s">
+      <c r="BE23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BE23" s="87" t="s">
+      <c r="BF23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BF23" s="91" t="s">
+      <c r="BG23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BG23" s="87" t="s">
+      <c r="BH23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BH23" s="91" t="s">
+      <c r="BI23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BI23" s="87" t="s">
+      <c r="BJ23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BJ23" s="91" t="s">
+      <c r="BK23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BK23" s="87" t="s">
+      <c r="BL23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BL23" s="91" t="s">
+      <c r="BM23" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="BM23" s="87" t="s">
+      <c r="BN23" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="BN23" s="38"/>
       <c r="BO23" s="38"/>
       <c r="BP23" s="38"/>
-      <c r="BQ23" s="122" t="s">
-        <v>206</v>
-      </c>
-      <c r="BR23" s="37"/>
+      <c r="BQ23" s="38"/>
+      <c r="BR23" s="118" t="s">
+        <v>205</v>
+      </c>
+      <c r="BS23" s="37"/>
     </row>
-    <row r="24" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="37"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -7981,61 +8026,75 @@
       <c r="AI24" s="18"/>
       <c r="AJ24" s="18"/>
       <c r="AK24" s="18"/>
-      <c r="AL24" s="18"/>
-      <c r="AM24" s="18"/>
-      <c r="AN24" s="18"/>
-      <c r="AO24" s="18"/>
-      <c r="AP24" s="142"/>
-      <c r="AQ24" s="18"/>
+      <c r="AL24" s="7">
+        <f>AN24*AO24*AS24</f>
+        <v>5</v>
+      </c>
+      <c r="AM24" s="7">
+        <f>AN24*AO24</f>
+        <v>1</v>
+      </c>
+      <c r="AN24" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO24" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP24" s="18"/>
+      <c r="AQ24" s="138"/>
       <c r="AR24" s="18"/>
-      <c r="AS24" s="18"/>
+      <c r="AS24" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AW24:$BN24)))))</f>
+        <v>5</v>
+      </c>
       <c r="AT24" s="18"/>
       <c r="AU24" s="18"/>
-      <c r="AV24" s="92"/>
-      <c r="AW24" s="7"/>
-      <c r="AX24" s="92" t="s">
+      <c r="AV24" s="18"/>
+      <c r="AW24" s="88"/>
+      <c r="AX24" s="7"/>
+      <c r="AY24" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AY24" s="7" t="s">
+      <c r="AZ24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AZ24" s="92" t="s">
+      <c r="BA24" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BA24" s="7" t="s">
+      <c r="BB24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BB24" s="92" t="s">
+      <c r="BC24" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BC24" s="7" t="s">
+      <c r="BD24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BD24" s="92"/>
-      <c r="BE24" s="7"/>
-      <c r="BF24" s="92"/>
-      <c r="BG24" s="7"/>
-      <c r="BH24" s="92"/>
-      <c r="BI24" s="7"/>
-      <c r="BJ24" s="92" t="s">
+      <c r="BE24" s="88"/>
+      <c r="BF24" s="7"/>
+      <c r="BG24" s="88"/>
+      <c r="BH24" s="7"/>
+      <c r="BI24" s="88"/>
+      <c r="BJ24" s="7"/>
+      <c r="BK24" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BK24" s="7" t="s">
+      <c r="BL24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BL24" s="92" t="s">
+      <c r="BM24" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BM24" s="7" t="s">
+      <c r="BN24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BN24" s="38"/>
       <c r="BO24" s="38"/>
       <c r="BP24" s="38"/>
-      <c r="BQ24" s="18"/>
-      <c r="BR24" s="37"/>
+      <c r="BQ24" s="38"/>
+      <c r="BR24" s="18"/>
+      <c r="BS24" s="37"/>
     </row>
-    <row r="25" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="37"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -8074,67 +8133,81 @@
       <c r="AI25" s="18"/>
       <c r="AJ25" s="18"/>
       <c r="AK25" s="18"/>
-      <c r="AL25" s="18"/>
-      <c r="AM25" s="18"/>
-      <c r="AN25" s="18"/>
-      <c r="AO25" s="18"/>
-      <c r="AP25" s="142"/>
-      <c r="AQ25" s="18"/>
+      <c r="AL25" s="7">
+        <f>AN25*AO25*AS25</f>
+        <v>3</v>
+      </c>
+      <c r="AM25" s="7">
+        <f>AN25*AO25</f>
+        <v>1</v>
+      </c>
+      <c r="AN25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="18"/>
+      <c r="AQ25" s="138"/>
       <c r="AR25" s="18"/>
-      <c r="AS25" s="18"/>
+      <c r="AS25" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AW25:$BN25)))))</f>
+        <v>3</v>
+      </c>
       <c r="AT25" s="18"/>
       <c r="AU25" s="18"/>
-      <c r="AV25" s="92"/>
-      <c r="AW25" s="7"/>
-      <c r="AX25" s="92" t="s">
+      <c r="AV25" s="18"/>
+      <c r="AW25" s="88"/>
+      <c r="AX25" s="7"/>
+      <c r="AY25" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AY25" s="7" t="s">
+      <c r="AZ25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AZ25" s="92" t="s">
+      <c r="BA25" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BA25" s="7" t="s">
+      <c r="BB25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BB25" s="92" t="s">
+      <c r="BC25" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BC25" s="7" t="s">
+      <c r="BD25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BD25" s="92"/>
-      <c r="BE25" s="7"/>
-      <c r="BF25" s="92"/>
-      <c r="BG25" s="7"/>
-      <c r="BH25" s="92"/>
-      <c r="BI25" s="7"/>
-      <c r="BJ25" s="92" t="s">
+      <c r="BE25" s="88"/>
+      <c r="BF25" s="7"/>
+      <c r="BG25" s="88"/>
+      <c r="BH25" s="7"/>
+      <c r="BI25" s="88"/>
+      <c r="BJ25" s="7"/>
+      <c r="BK25" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="BK25" s="7" t="s">
+      <c r="BL25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BL25" s="92" t="s">
+      <c r="BM25" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="BM25" s="7" t="s">
+      <c r="BN25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BN25" s="38"/>
       <c r="BO25" s="38"/>
       <c r="BP25" s="38"/>
-      <c r="BQ25" s="18"/>
-      <c r="BR25" s="37"/>
+      <c r="BQ25" s="38"/>
+      <c r="BR25" s="18"/>
+      <c r="BS25" s="37"/>
     </row>
-    <row r="26" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="37"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
@@ -8167,51 +8240,65 @@
       <c r="AI26" s="18"/>
       <c r="AJ26" s="18"/>
       <c r="AK26" s="18"/>
-      <c r="AL26" s="18"/>
-      <c r="AM26" s="18"/>
-      <c r="AN26" s="18"/>
-      <c r="AO26" s="18"/>
-      <c r="AP26" s="142"/>
-      <c r="AQ26" s="18"/>
+      <c r="AL26" s="7">
+        <f>AN26*AO26*AS26</f>
+        <v>1</v>
+      </c>
+      <c r="AM26" s="7">
+        <f>AN26*AO26</f>
+        <v>1</v>
+      </c>
+      <c r="AN26" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO26" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="18"/>
+      <c r="AQ26" s="138"/>
       <c r="AR26" s="18"/>
-      <c r="AS26" s="18"/>
+      <c r="AS26" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AW26:$BN26)))))</f>
+        <v>1</v>
+      </c>
       <c r="AT26" s="18"/>
       <c r="AU26" s="18"/>
-      <c r="AV26" s="92" t="s">
+      <c r="AV26" s="18"/>
+      <c r="AW26" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AW26" s="7" t="s">
+      <c r="AX26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AX26" s="92"/>
-      <c r="AY26" s="7"/>
-      <c r="AZ26" s="92"/>
-      <c r="BA26" s="7"/>
-      <c r="BB26" s="92"/>
-      <c r="BC26" s="7"/>
-      <c r="BD26" s="92"/>
-      <c r="BE26" s="7"/>
-      <c r="BF26" s="92"/>
-      <c r="BG26" s="7"/>
-      <c r="BH26" s="92"/>
-      <c r="BI26" s="7"/>
-      <c r="BJ26" s="92"/>
-      <c r="BK26" s="7"/>
-      <c r="BL26" s="92"/>
-      <c r="BM26" s="7"/>
-      <c r="BN26" s="38"/>
+      <c r="AY26" s="88"/>
+      <c r="AZ26" s="7"/>
+      <c r="BA26" s="88"/>
+      <c r="BB26" s="7"/>
+      <c r="BC26" s="88"/>
+      <c r="BD26" s="7"/>
+      <c r="BE26" s="88"/>
+      <c r="BF26" s="7"/>
+      <c r="BG26" s="88"/>
+      <c r="BH26" s="7"/>
+      <c r="BI26" s="88"/>
+      <c r="BJ26" s="7"/>
+      <c r="BK26" s="88"/>
+      <c r="BL26" s="7"/>
+      <c r="BM26" s="88"/>
+      <c r="BN26" s="7"/>
       <c r="BO26" s="38"/>
       <c r="BP26" s="38"/>
-      <c r="BQ26" s="18"/>
-      <c r="BR26" s="37"/>
+      <c r="BQ26" s="38"/>
+      <c r="BR26" s="18"/>
+      <c r="BS26" s="37"/>
     </row>
-    <row r="27" spans="2:70" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:71" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="4"/>
       <c r="C27" s="18"/>
       <c r="D27" s="58"/>
       <c r="E27" s="18"/>
       <c r="F27" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>150</v>
@@ -8272,73 +8359,87 @@
       <c r="AI27" s="7"/>
       <c r="AJ27" s="16"/>
       <c r="AK27" s="7"/>
-      <c r="AL27" s="7"/>
-      <c r="AM27" s="7"/>
-      <c r="AN27" s="7"/>
-      <c r="AO27" s="7"/>
-      <c r="AP27" s="140"/>
-      <c r="AQ27" s="7"/>
+      <c r="AL27" s="7">
+        <f>AN27*AO27*AS27</f>
+        <v>6</v>
+      </c>
+      <c r="AM27" s="7">
+        <f>AN27*AO27</f>
+        <v>1</v>
+      </c>
+      <c r="AN27" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO27" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="7"/>
+      <c r="AQ27" s="136"/>
       <c r="AR27" s="7"/>
-      <c r="AS27" s="7"/>
+      <c r="AS27" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AW27:$BN27)))))</f>
+        <v>6</v>
+      </c>
       <c r="AT27" s="7"/>
       <c r="AU27" s="7"/>
-      <c r="AV27" s="92" t="s">
+      <c r="AV27" s="7"/>
+      <c r="AW27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AW27" s="7" t="s">
+      <c r="AX27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AX27" s="92" t="s">
+      <c r="AY27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AY27" s="7" t="s">
+      <c r="AZ27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AZ27" s="92" t="s">
+      <c r="BA27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BA27" s="7" t="s">
+      <c r="BB27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BB27" s="92" t="s">
+      <c r="BC27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BC27" s="7" t="s">
+      <c r="BD27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BD27" s="92"/>
-      <c r="BE27" s="7"/>
-      <c r="BF27" s="92"/>
-      <c r="BG27" s="7"/>
-      <c r="BH27" s="92"/>
-      <c r="BI27" s="7"/>
-      <c r="BJ27" s="92" t="s">
+      <c r="BE27" s="88"/>
+      <c r="BF27" s="7"/>
+      <c r="BG27" s="88"/>
+      <c r="BH27" s="7"/>
+      <c r="BI27" s="88"/>
+      <c r="BJ27" s="7"/>
+      <c r="BK27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BK27" s="7" t="s">
+      <c r="BL27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BL27" s="92" t="s">
+      <c r="BM27" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BM27" s="7" t="s">
+      <c r="BN27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BN27" s="16"/>
-      <c r="BO27" s="7"/>
+      <c r="BO27" s="16"/>
       <c r="BP27" s="7"/>
-      <c r="BQ27" s="18" t="s">
+      <c r="BQ27" s="7"/>
+      <c r="BR27" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="BR27" s="12"/>
+      <c r="BS27" s="12"/>
     </row>
-    <row r="28" spans="2:70" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:71" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="4"/>
       <c r="C28" s="18"/>
       <c r="D28" s="58"/>
       <c r="E28" s="18"/>
       <c r="F28" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="16"/>
@@ -8371,163 +8472,178 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="16"/>
       <c r="AK28" s="7"/>
-      <c r="AL28" s="7"/>
-      <c r="AM28" s="7"/>
-      <c r="AN28" s="7"/>
-      <c r="AO28" s="7"/>
-      <c r="AP28" s="140"/>
-      <c r="AQ28" s="7"/>
+      <c r="AL28" s="7">
+        <f>AN28*AO28*AS28</f>
+        <v>4</v>
+      </c>
+      <c r="AM28" s="7">
+        <f>AN28*AO28</f>
+        <v>1</v>
+      </c>
+      <c r="AN28" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO28" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP28" s="7"/>
+      <c r="AQ28" s="136"/>
       <c r="AR28" s="7"/>
-      <c r="AS28" s="7"/>
+      <c r="AS28" s="7">
+        <f>SUMPRODUCT(--(ISNUMBER(FIND(AS$10,UPPER($AW28:$BN28)))))</f>
+        <v>4</v>
+      </c>
       <c r="AT28" s="7"/>
       <c r="AU28" s="7"/>
-      <c r="AV28" s="92" t="s">
+      <c r="AV28" s="7"/>
+      <c r="AW28" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="AW28" s="7" t="s">
+      <c r="AX28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AX28" s="92" t="s">
+      <c r="AY28" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AY28" s="7" t="s">
+      <c r="AZ28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AZ28" s="92" t="s">
+      <c r="BA28" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BA28" s="7" t="s">
+      <c r="BB28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BB28" s="92" t="s">
+      <c r="BC28" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BC28" s="7" t="s">
+      <c r="BD28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BD28" s="92"/>
-      <c r="BE28" s="7"/>
-      <c r="BF28" s="92"/>
-      <c r="BG28" s="7"/>
-      <c r="BH28" s="92" t="s">
+      <c r="BE28" s="88"/>
+      <c r="BF28" s="7"/>
+      <c r="BG28" s="88"/>
+      <c r="BH28" s="7"/>
+      <c r="BI28" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="BI28" s="7" t="s">
+      <c r="BJ28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BJ28" s="92"/>
-      <c r="BK28" s="7"/>
-      <c r="BL28" s="92"/>
-      <c r="BM28" s="7"/>
-      <c r="BN28" s="16"/>
-      <c r="BO28" s="7"/>
+      <c r="BK28" s="88"/>
+      <c r="BL28" s="7"/>
+      <c r="BM28" s="88"/>
+      <c r="BN28" s="7"/>
+      <c r="BO28" s="16"/>
       <c r="BP28" s="7"/>
-      <c r="BQ28" s="18"/>
-      <c r="BR28" s="8"/>
+      <c r="BQ28" s="7"/>
+      <c r="BR28" s="18"/>
+      <c r="BS28" s="8"/>
     </row>
-    <row r="29" spans="2:70" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="92" t="s">
+    <row r="29" spans="2:71" s="84" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C29" s="115"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="G29" s="92" t="s">
+      <c r="G29" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92" t="s">
+      <c r="H29" s="88"/>
+      <c r="I29" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92" t="s">
+      <c r="J29" s="88"/>
+      <c r="K29" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="L29" s="92" t="s">
+      <c r="L29" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92" t="s">
+      <c r="M29" s="88"/>
+      <c r="N29" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="O29" s="92"/>
-      <c r="P29" s="92"/>
-      <c r="Q29" s="92"/>
-      <c r="R29" s="92"/>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92" t="s">
+      <c r="O29" s="88"/>
+      <c r="P29" s="88"/>
+      <c r="Q29" s="88"/>
+      <c r="R29" s="88"/>
+      <c r="S29" s="88"/>
+      <c r="T29" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="U29" s="92"/>
-      <c r="V29" s="92" t="s">
+      <c r="U29" s="88"/>
+      <c r="V29" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="W29" s="92"/>
-      <c r="X29" s="92"/>
-      <c r="Y29" s="92"/>
-      <c r="Z29" s="92" t="s">
+      <c r="W29" s="88"/>
+      <c r="X29" s="88"/>
+      <c r="Y29" s="88"/>
+      <c r="Z29" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="AA29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF29" s="121" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG29" s="92"/>
-      <c r="AH29" s="92"/>
-      <c r="AI29" s="92"/>
-      <c r="AJ29" s="92"/>
-      <c r="AK29" s="92"/>
-      <c r="AL29" s="92"/>
-      <c r="AM29" s="92"/>
-      <c r="AN29" s="92"/>
-      <c r="AO29" s="92"/>
-      <c r="AP29" s="140"/>
-      <c r="AQ29" s="92"/>
-      <c r="AR29" s="92"/>
-      <c r="AS29" s="92"/>
-      <c r="AT29" s="92"/>
-      <c r="AU29" s="92"/>
-      <c r="AV29" s="92"/>
-      <c r="AW29" s="92"/>
-      <c r="AX29" s="114"/>
-      <c r="AY29" s="92"/>
-      <c r="AZ29" s="92"/>
-      <c r="BA29" s="92"/>
-      <c r="BB29" s="92"/>
-      <c r="BC29" s="92"/>
-      <c r="BD29" s="92"/>
-      <c r="BE29" s="92"/>
-      <c r="BF29" s="92"/>
-      <c r="BG29" s="92"/>
-      <c r="BH29" s="92"/>
-      <c r="BI29" s="92"/>
-      <c r="BJ29" s="92"/>
-      <c r="BK29" s="92"/>
-      <c r="BL29" s="92"/>
-      <c r="BM29" s="92"/>
-      <c r="BN29" s="92"/>
-      <c r="BO29" s="92"/>
-      <c r="BP29" s="92"/>
-      <c r="BQ29" s="120" t="s">
+      <c r="AA29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF29" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG29" s="88"/>
+      <c r="AH29" s="88"/>
+      <c r="AI29" s="88"/>
+      <c r="AJ29" s="88"/>
+      <c r="AK29" s="88"/>
+      <c r="AL29" s="88"/>
+      <c r="AM29" s="88"/>
+      <c r="AN29" s="88"/>
+      <c r="AO29" s="88"/>
+      <c r="AP29" s="88"/>
+      <c r="AQ29" s="136"/>
+      <c r="AR29" s="88"/>
+      <c r="AS29" s="88"/>
+      <c r="AT29" s="88"/>
+      <c r="AU29" s="88"/>
+      <c r="AV29" s="88"/>
+      <c r="AW29" s="88"/>
+      <c r="AX29" s="88"/>
+      <c r="AY29" s="110"/>
+      <c r="AZ29" s="88"/>
+      <c r="BA29" s="88"/>
+      <c r="BB29" s="88"/>
+      <c r="BC29" s="88"/>
+      <c r="BD29" s="88"/>
+      <c r="BE29" s="88"/>
+      <c r="BF29" s="88"/>
+      <c r="BG29" s="88"/>
+      <c r="BH29" s="88"/>
+      <c r="BI29" s="88"/>
+      <c r="BJ29" s="88"/>
+      <c r="BK29" s="88"/>
+      <c r="BL29" s="88"/>
+      <c r="BM29" s="88"/>
+      <c r="BN29" s="88"/>
+      <c r="BO29" s="88"/>
+      <c r="BP29" s="88"/>
+      <c r="BQ29" s="88"/>
+      <c r="BR29" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="BR29" s="90"/>
+      <c r="BS29" s="86"/>
     </row>
-    <row r="30" spans="2:70" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:71" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="37"/>
       <c r="C30" s="52"/>
       <c r="D30" s="52"/>
@@ -8568,192 +8684,192 @@
       <c r="AM30" s="38"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="38"/>
-      <c r="AP30" s="140"/>
-      <c r="AQ30" s="38"/>
+      <c r="AP30" s="38"/>
+      <c r="AQ30" s="136"/>
       <c r="AR30" s="38"/>
       <c r="AS30" s="38"/>
       <c r="AT30" s="38"/>
       <c r="AU30" s="38"/>
-      <c r="AV30" s="92"/>
-      <c r="AW30" s="38"/>
-      <c r="AX30" s="114"/>
-      <c r="AY30" s="38"/>
-      <c r="AZ30" s="92"/>
-      <c r="BA30" s="38"/>
-      <c r="BB30" s="92"/>
-      <c r="BC30" s="38"/>
-      <c r="BD30" s="92"/>
-      <c r="BE30" s="38"/>
-      <c r="BF30" s="92"/>
-      <c r="BG30" s="38"/>
-      <c r="BH30" s="92"/>
-      <c r="BI30" s="38"/>
-      <c r="BJ30" s="92"/>
-      <c r="BK30" s="38"/>
-      <c r="BL30" s="92"/>
-      <c r="BM30" s="38"/>
+      <c r="AV30" s="38"/>
+      <c r="AW30" s="88"/>
+      <c r="AX30" s="38"/>
+      <c r="AY30" s="110"/>
+      <c r="AZ30" s="38"/>
+      <c r="BA30" s="88"/>
+      <c r="BB30" s="38"/>
+      <c r="BC30" s="88"/>
+      <c r="BD30" s="38"/>
+      <c r="BE30" s="88"/>
+      <c r="BF30" s="38"/>
+      <c r="BG30" s="88"/>
+      <c r="BH30" s="38"/>
+      <c r="BI30" s="88"/>
+      <c r="BJ30" s="38"/>
+      <c r="BK30" s="88"/>
+      <c r="BL30" s="38"/>
+      <c r="BM30" s="88"/>
       <c r="BN30" s="38"/>
       <c r="BO30" s="38"/>
       <c r="BP30" s="38"/>
       <c r="BQ30" s="38"/>
-      <c r="BR30" s="37"/>
+      <c r="BR30" s="38"/>
+      <c r="BS30" s="37"/>
     </row>
-    <row r="31" spans="2:70" s="134" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="123"/>
-      <c r="C31" s="124" t="s">
+    <row r="31" spans="2:71" s="130" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="119"/>
+      <c r="C31" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="124"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="126" t="s">
+      <c r="D31" s="120"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122" t="s">
         <v>147</v>
       </c>
-      <c r="H31" s="127" t="s">
+      <c r="H31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="I31" s="128" t="s">
+      <c r="I31" s="124" t="s">
         <v>125</v>
       </c>
-      <c r="J31" s="127" t="s">
+      <c r="J31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="K31" s="128" t="s">
+      <c r="K31" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="L31" s="128" t="s">
+      <c r="L31" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="M31" s="127" t="s">
+      <c r="M31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="N31" s="128" t="s">
+      <c r="N31" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="O31" s="128" t="s">
+      <c r="O31" s="124" t="s">
         <v>137</v>
       </c>
-      <c r="P31" s="128" t="s">
+      <c r="P31" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="Q31" s="128" t="s">
+      <c r="Q31" s="124" t="s">
         <v>139</v>
       </c>
-      <c r="R31" s="128" t="s">
+      <c r="R31" s="124" t="s">
         <v>140</v>
       </c>
-      <c r="S31" s="127" t="s">
+      <c r="S31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="T31" s="128" t="s">
+      <c r="T31" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="U31" s="127" t="s">
+      <c r="U31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="V31" s="128" t="s">
+      <c r="V31" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="W31" s="128" t="s">
+      <c r="W31" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="X31" s="127" t="s">
+      <c r="X31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="Y31" s="129" t="s">
+      <c r="Y31" s="125" t="s">
         <v>142</v>
       </c>
-      <c r="Z31" s="128" t="s">
+      <c r="Z31" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="AA31" s="128" t="s">
+      <c r="AA31" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="AB31" s="128" t="s">
+      <c r="AB31" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="AC31" s="128" t="s">
+      <c r="AC31" s="124" t="s">
         <v>102</v>
       </c>
-      <c r="AD31" s="128" t="s">
+      <c r="AD31" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="AE31" s="128" t="s">
+      <c r="AE31" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="AF31" s="128" t="s">
+      <c r="AF31" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="AG31" s="127" t="s">
+      <c r="AG31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="AH31" s="130" t="s">
+      <c r="AH31" s="126" t="s">
         <v>95</v>
       </c>
-      <c r="AI31" s="128"/>
-      <c r="AJ31" s="127" t="s">
+      <c r="AI31" s="124"/>
+      <c r="AJ31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="AK31" s="129" t="s">
+      <c r="AK31" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="AL31" s="129"/>
-      <c r="AM31" s="129" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN31" s="129" t="s">
+      <c r="AL31" s="125"/>
+      <c r="AM31" s="125"/>
+      <c r="AN31" s="125"/>
+      <c r="AO31" s="125" t="s">
         <v>195</v>
       </c>
-      <c r="AO31" s="129"/>
-      <c r="AP31" s="143"/>
-      <c r="AQ31" s="129"/>
-      <c r="AR31" s="129"/>
-      <c r="AS31" s="129"/>
-      <c r="AT31" s="129"/>
-      <c r="AU31" s="128"/>
-      <c r="AV31" s="131" t="s">
+      <c r="AP31" s="125"/>
+      <c r="AQ31" s="139"/>
+      <c r="AR31" s="125"/>
+      <c r="AS31" s="125"/>
+      <c r="AT31" s="125"/>
+      <c r="AU31" s="125"/>
+      <c r="AV31" s="124"/>
+      <c r="AW31" s="127" t="s">
         <v>172</v>
       </c>
-      <c r="AW31" s="128"/>
-      <c r="AX31" s="132" t="s">
+      <c r="AX31" s="124"/>
+      <c r="AY31" s="128" t="s">
         <v>174</v>
       </c>
-      <c r="AY31" s="128"/>
-      <c r="AZ31" s="131" t="s">
+      <c r="AZ31" s="124"/>
+      <c r="BA31" s="127" t="s">
         <v>175</v>
       </c>
-      <c r="BA31" s="128"/>
-      <c r="BB31" s="131" t="s">
+      <c r="BB31" s="124"/>
+      <c r="BC31" s="127" t="s">
         <v>176</v>
       </c>
-      <c r="BC31" s="128"/>
-      <c r="BD31" s="131" t="s">
+      <c r="BD31" s="124"/>
+      <c r="BE31" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="BE31" s="128"/>
-      <c r="BF31" s="131" t="s">
+      <c r="BF31" s="124"/>
+      <c r="BG31" s="127" t="s">
         <v>170</v>
       </c>
-      <c r="BG31" s="128"/>
-      <c r="BH31" s="131" t="s">
+      <c r="BH31" s="124"/>
+      <c r="BI31" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="BI31" s="128"/>
-      <c r="BJ31" s="131" t="s">
+      <c r="BJ31" s="124"/>
+      <c r="BK31" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="BK31" s="128"/>
-      <c r="BL31" s="131" t="s">
+      <c r="BL31" s="124"/>
+      <c r="BM31" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="BM31" s="128"/>
-      <c r="BN31" s="127" t="s">
+      <c r="BN31" s="124"/>
+      <c r="BO31" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="BO31" s="128"/>
-      <c r="BP31" s="128"/>
-      <c r="BQ31" s="125"/>
-      <c r="BR31" s="133"/>
+      <c r="BP31" s="124"/>
+      <c r="BQ31" s="124"/>
+      <c r="BR31" s="121"/>
+      <c r="BS31" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8771,49 +8887,49 @@
   <dimension ref="B4:AZ82"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F55" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AI74" sqref="AI74"/>
+      <selection pane="bottomRight" activeCell="M74" sqref="M74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="9" style="9"/>
-    <col min="2" max="2" width="2.59765625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="3.73046875" style="56" customWidth="1"/>
-    <col min="4" max="4" width="11.06640625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="2.578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="3.734375" style="56" customWidth="1"/>
+    <col min="4" max="4" width="11.05078125" style="56" customWidth="1"/>
     <col min="5" max="6" width="25" style="9" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="3.59765625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="3.59765625" style="19" customWidth="1"/>
-    <col min="10" max="11" width="3.59765625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="3.59765625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="3.59765625" style="9" customWidth="1"/>
-    <col min="14" max="17" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="3.59765625" style="19" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="3.59765625" style="9" customWidth="1"/>
-    <col min="20" max="20" width="3.59765625" style="19" customWidth="1"/>
-    <col min="21" max="22" width="3.59765625" style="9" customWidth="1"/>
-    <col min="23" max="23" width="3.59765625" style="19" customWidth="1"/>
-    <col min="24" max="24" width="3.59765625" style="9" customWidth="1"/>
-    <col min="25" max="31" width="3.59765625" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="3.59765625" style="19" customWidth="1" collapsed="1"/>
-    <col min="33" max="34" width="3.59765625" style="9" customWidth="1"/>
-    <col min="35" max="35" width="3.59765625" style="19" customWidth="1"/>
-    <col min="36" max="36" width="3.59765625" style="9" customWidth="1"/>
-    <col min="37" max="46" width="3.59765625" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="3.59765625" style="19" customWidth="1"/>
-    <col min="48" max="49" width="3.59765625" style="9" customWidth="1"/>
-    <col min="50" max="50" width="25.33203125" style="9" customWidth="1"/>
-    <col min="51" max="51" width="73.265625" style="9" customWidth="1"/>
-    <col min="52" max="52" width="2.59765625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="3.578125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="3.578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="3.578125" style="19" customWidth="1"/>
+    <col min="10" max="11" width="3.578125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="3.578125" style="19" customWidth="1"/>
+    <col min="13" max="13" width="3.578125" style="9" customWidth="1"/>
+    <col min="14" max="17" width="3.578125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="3.578125" style="19" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="3.578125" style="9" customWidth="1"/>
+    <col min="20" max="20" width="3.578125" style="19" customWidth="1"/>
+    <col min="21" max="22" width="3.578125" style="9" customWidth="1"/>
+    <col min="23" max="23" width="3.578125" style="19" customWidth="1"/>
+    <col min="24" max="24" width="3.578125" style="9" customWidth="1"/>
+    <col min="25" max="31" width="3.578125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="3.578125" style="19" customWidth="1" collapsed="1"/>
+    <col min="33" max="34" width="3.578125" style="9" customWidth="1"/>
+    <col min="35" max="35" width="3.578125" style="19" customWidth="1"/>
+    <col min="36" max="36" width="3.578125" style="9" customWidth="1"/>
+    <col min="37" max="46" width="3.578125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="3.578125" style="19" customWidth="1"/>
+    <col min="48" max="49" width="3.578125" style="9" customWidth="1"/>
+    <col min="50" max="50" width="25.3125" style="9" customWidth="1"/>
+    <col min="51" max="51" width="73.26171875" style="9" customWidth="1"/>
+    <col min="52" max="52" width="2.578125" style="9" customWidth="1"/>
     <col min="53" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:52" outlineLevel="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:52" outlineLevel="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="5" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="37"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -8866,7 +8982,7 @@
       <c r="AY5" s="37"/>
       <c r="AZ5" s="37"/>
     </row>
-    <row r="6" spans="2:52" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:52" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4"/>
       <c r="C6" s="49" t="s">
         <v>0</v>
@@ -8919,7 +9035,7 @@
       <c r="AY6" s="11"/>
       <c r="AZ6" s="12"/>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4"/>
       <c r="C7" s="50"/>
       <c r="D7" s="50"/>
@@ -8972,7 +9088,7 @@
       <c r="AY7" s="14"/>
       <c r="AZ7" s="12"/>
     </row>
-    <row r="8" spans="2:52" s="24" customFormat="1" ht="127.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:52" s="24" customFormat="1" ht="128.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="20"/>
       <c r="C8" s="57" t="s">
         <v>67</v>
@@ -9105,7 +9221,7 @@
       <c r="AY8" s="22"/>
       <c r="AZ8" s="23"/>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51"/>
@@ -9132,14 +9248,14 @@
       <c r="U9" s="42"/>
       <c r="V9" s="42"/>
       <c r="W9" s="42"/>
-      <c r="X9" s="84"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="85"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="86"/>
+      <c r="X9" s="140"/>
+      <c r="Y9" s="141"/>
+      <c r="Z9" s="141"/>
+      <c r="AA9" s="141"/>
+      <c r="AB9" s="141"/>
+      <c r="AC9" s="141"/>
+      <c r="AD9" s="141"/>
+      <c r="AE9" s="142"/>
       <c r="AF9" s="42"/>
       <c r="AG9" s="43"/>
       <c r="AH9" s="42"/>
@@ -9166,7 +9282,7 @@
       </c>
       <c r="AZ9" s="12"/>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="37"/>
       <c r="C10" s="52"/>
       <c r="D10" s="52"/>
@@ -9219,7 +9335,7 @@
       <c r="AY10" s="38"/>
       <c r="AZ10" s="37"/>
     </row>
-    <row r="11" spans="2:52" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:52" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4"/>
       <c r="C11" s="78"/>
       <c r="D11" s="78"/>
@@ -9286,7 +9402,7 @@
       </c>
       <c r="AZ11" s="12"/>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="37"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
@@ -9339,7 +9455,7 @@
       <c r="AY12" s="38"/>
       <c r="AZ12" s="37"/>
     </row>
-    <row r="13" spans="2:52" ht="228" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:52" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4"/>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
@@ -9400,7 +9516,7 @@
       </c>
       <c r="AZ13" s="8"/>
     </row>
-    <row r="14" spans="2:52" ht="42.75" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:52" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4"/>
       <c r="C14" s="58" t="s">
         <v>28</v>
@@ -9497,7 +9613,7 @@
       <c r="AY14" s="17"/>
       <c r="AZ14" s="12"/>
     </row>
-    <row r="15" spans="2:52" ht="42.75" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:52" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4"/>
       <c r="C15" s="58" t="s">
         <v>28</v>
@@ -9594,7 +9710,7 @@
       <c r="AY15" s="17"/>
       <c r="AZ15" s="12"/>
     </row>
-    <row r="16" spans="2:52" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:52" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4"/>
       <c r="C16" s="53"/>
       <c r="D16" s="53"/>
@@ -9649,7 +9765,7 @@
       <c r="AY16" s="17"/>
       <c r="AZ16" s="12"/>
     </row>
-    <row r="17" spans="2:52" ht="42.75" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:52" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4"/>
       <c r="C17" s="59" t="s">
         <v>34</v>
@@ -9750,7 +9866,7 @@
       <c r="AY17" s="17"/>
       <c r="AZ17" s="12"/>
     </row>
-    <row r="18" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="37"/>
       <c r="C18" s="52"/>
       <c r="D18" s="52"/>
@@ -9803,7 +9919,7 @@
       <c r="AY18" s="38"/>
       <c r="AZ18" s="37"/>
     </row>
-    <row r="19" spans="2:52" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:52" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
@@ -9878,7 +9994,7 @@
       </c>
       <c r="AZ19" s="12"/>
     </row>
-    <row r="20" spans="2:52" ht="48" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:52" ht="48" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4"/>
       <c r="C20" s="53" t="s">
         <v>16</v>
@@ -9977,7 +10093,7 @@
       </c>
       <c r="AZ20" s="12"/>
     </row>
-    <row r="21" spans="2:52" ht="48.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:52" ht="48.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4"/>
       <c r="C21" s="58" t="s">
         <v>28</v>
@@ -10074,7 +10190,7 @@
       </c>
       <c r="AZ21" s="12"/>
     </row>
-    <row r="22" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4"/>
       <c r="C22" s="58" t="s">
         <v>28</v>
@@ -10175,7 +10291,7 @@
       </c>
       <c r="AZ22" s="12"/>
     </row>
-    <row r="23" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="4"/>
       <c r="C23" s="59" t="s">
         <v>34</v>
@@ -10276,7 +10392,7 @@
       </c>
       <c r="AZ23" s="12"/>
     </row>
-    <row r="24" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="4"/>
       <c r="C24" s="59" t="s">
         <v>34</v>
@@ -10371,7 +10487,7 @@
       </c>
       <c r="AZ24" s="8"/>
     </row>
-    <row r="25" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="4"/>
       <c r="C25" s="59" t="s">
         <v>34</v>
@@ -10466,7 +10582,7 @@
       </c>
       <c r="AZ25" s="8"/>
     </row>
-    <row r="26" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="4"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -10524,7 +10640,7 @@
       </c>
       <c r="AZ26" s="8"/>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="4"/>
       <c r="C27" s="53"/>
       <c r="D27" s="53"/>
@@ -10577,7 +10693,7 @@
       <c r="AY27" s="17"/>
       <c r="AZ27" s="8"/>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="37"/>
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
@@ -10630,7 +10746,7 @@
       <c r="AY28" s="38"/>
       <c r="AZ28" s="37"/>
     </row>
-    <row r="29" spans="2:52" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:52" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="4"/>
       <c r="C29" s="53"/>
       <c r="D29" s="53"/>
@@ -10697,7 +10813,7 @@
       </c>
       <c r="AZ29" s="12"/>
     </row>
-    <row r="30" spans="2:52" ht="42.75" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:52" ht="43.2" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="4"/>
       <c r="C30" s="53" t="s">
         <v>16</v>
@@ -10772,7 +10888,7 @@
       </c>
       <c r="AZ30" s="12"/>
     </row>
-    <row r="31" spans="2:52" ht="42.75" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:52" ht="43.2" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="4"/>
       <c r="C31" s="58" t="s">
         <v>28</v>
@@ -10871,7 +10987,7 @@
       </c>
       <c r="AZ31" s="12"/>
     </row>
-    <row r="32" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="4"/>
       <c r="C32" s="59" t="s">
         <v>34</v>
@@ -10968,7 +11084,7 @@
       </c>
       <c r="AZ32" s="12"/>
     </row>
-    <row r="33" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="4"/>
       <c r="C33" s="59" t="s">
         <v>34</v>
@@ -11069,7 +11185,7 @@
       </c>
       <c r="AZ33" s="12"/>
     </row>
-    <row r="34" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="4"/>
       <c r="C34" s="58" t="s">
         <v>28</v>
@@ -11170,7 +11286,7 @@
       </c>
       <c r="AZ34" s="12"/>
     </row>
-    <row r="35" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="4"/>
       <c r="C35" s="59" t="s">
         <v>34</v>
@@ -11265,7 +11381,7 @@
       </c>
       <c r="AZ35" s="8"/>
     </row>
-    <row r="36" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:52" outlineLevel="3" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="4"/>
       <c r="C36" s="53"/>
       <c r="D36" s="53"/>
@@ -11358,7 +11474,7 @@
       </c>
       <c r="AZ36" s="8"/>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="4"/>
       <c r="C37" s="53"/>
       <c r="D37" s="53"/>
@@ -11411,7 +11527,7 @@
       <c r="AY37" s="17"/>
       <c r="AZ37" s="8"/>
     </row>
-    <row r="38" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="37"/>
       <c r="C38" s="52"/>
       <c r="D38" s="52"/>
@@ -11464,7 +11580,7 @@
       <c r="AY38" s="70"/>
       <c r="AZ38" s="37"/>
     </row>
-    <row r="39" spans="2:52" ht="116.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:52" ht="116.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="4"/>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
@@ -11523,7 +11639,7 @@
       </c>
       <c r="AZ39" s="12"/>
     </row>
-    <row r="40" spans="2:52" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:52" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="4"/>
       <c r="C40" s="54"/>
       <c r="D40" s="54"/>
@@ -11595,7 +11711,7 @@
       <c r="AY40" s="15"/>
       <c r="AZ40" s="12"/>
     </row>
-    <row r="41" spans="2:52" ht="28.5" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:52" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="4"/>
       <c r="C41" s="58" t="s">
         <v>28</v>
@@ -11689,7 +11805,7 @@
       </c>
       <c r="AZ41" s="12"/>
     </row>
-    <row r="42" spans="2:52" ht="28.5" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:52" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="4"/>
       <c r="C42" s="58" t="s">
         <v>28</v>
@@ -11776,12 +11892,12 @@
       <c r="AV42" s="26"/>
       <c r="AW42" s="26"/>
       <c r="AX42" s="72"/>
-      <c r="AY42" s="82" t="s">
+      <c r="AY42" s="143" t="s">
         <v>36</v>
       </c>
       <c r="AZ42" s="12"/>
     </row>
-    <row r="43" spans="2:52" ht="28.5" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:52" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="4"/>
       <c r="C43" s="58" t="s">
         <v>28</v>
@@ -11870,10 +11986,10 @@
       <c r="AV43" s="26"/>
       <c r="AW43" s="26"/>
       <c r="AX43" s="73"/>
-      <c r="AY43" s="83"/>
+      <c r="AY43" s="144"/>
       <c r="AZ43" s="12"/>
     </row>
-    <row r="44" spans="2:52" ht="28.5" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:52" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="4"/>
       <c r="C44" s="59" t="s">
         <v>34</v>
@@ -11963,7 +12079,7 @@
       <c r="AY44" s="15"/>
       <c r="AZ44" s="12"/>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="4"/>
       <c r="C45" s="59"/>
       <c r="D45" s="54"/>
@@ -12015,7 +12131,7 @@
       <c r="AY45" s="15"/>
       <c r="AZ45" s="12"/>
     </row>
-    <row r="46" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="4"/>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -12068,7 +12184,7 @@
       <c r="AY46" s="36"/>
       <c r="AZ46" s="12"/>
     </row>
-    <row r="47" spans="2:52" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:52" ht="92.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="4"/>
       <c r="C47" s="54"/>
       <c r="D47" s="54"/>
@@ -12136,7 +12252,7 @@
       </c>
       <c r="AZ47" s="12"/>
     </row>
-    <row r="48" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="4"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -12196,7 +12312,7 @@
       </c>
       <c r="AZ48" s="8"/>
     </row>
-    <row r="49" spans="2:52" ht="28.5" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:52" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="4"/>
       <c r="C49" s="58" t="s">
         <v>28</v>
@@ -12288,7 +12404,7 @@
       <c r="AY49" s="67"/>
       <c r="AZ49" s="12"/>
     </row>
-    <row r="50" spans="2:52" ht="28.5" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:52" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="4"/>
       <c r="C50" s="58" t="s">
         <v>28</v>
@@ -12380,7 +12496,7 @@
       <c r="AY50" s="67"/>
       <c r="AZ50" s="12"/>
     </row>
-    <row r="51" spans="2:52" ht="28.5" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:52" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="4"/>
       <c r="C51" s="59" t="s">
         <v>34</v>
@@ -12470,7 +12586,7 @@
       <c r="AY51" s="15"/>
       <c r="AZ51" s="12"/>
     </row>
-    <row r="52" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="4"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -12530,7 +12646,7 @@
       </c>
       <c r="AZ52" s="8"/>
     </row>
-    <row r="53" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="4"/>
       <c r="C53" s="59"/>
       <c r="D53" s="54"/>
@@ -12582,7 +12698,7 @@
       <c r="AY53" s="15"/>
       <c r="AZ53" s="12"/>
     </row>
-    <row r="54" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="37"/>
       <c r="C54" s="52"/>
       <c r="D54" s="52"/>
@@ -12635,7 +12751,7 @@
       <c r="AY54" s="38"/>
       <c r="AZ54" s="37"/>
     </row>
-    <row r="55" spans="2:52" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:52" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="4"/>
       <c r="C55" s="53"/>
       <c r="D55" s="53"/>
@@ -12718,7 +12834,7 @@
       </c>
       <c r="AZ55" s="12"/>
     </row>
-    <row r="56" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="4"/>
       <c r="C56" s="59" t="s">
         <v>34</v>
@@ -12805,7 +12921,7 @@
       <c r="AY56" s="18"/>
       <c r="AZ56" s="8"/>
     </row>
-    <row r="57" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:52" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="4"/>
       <c r="C57" s="59" t="s">
         <v>34</v>
@@ -12880,7 +12996,7 @@
       <c r="AY57" s="18"/>
       <c r="AZ57" s="8"/>
     </row>
-    <row r="58" spans="2:52" ht="42.75" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:52" ht="43.2" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="4"/>
       <c r="C58" s="58" t="s">
         <v>28</v>
@@ -12957,7 +13073,7 @@
       </c>
       <c r="AZ58" s="8"/>
     </row>
-    <row r="59" spans="2:52" ht="28.5" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:52" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="4"/>
       <c r="C59" s="53" t="s">
         <v>27</v>
@@ -13034,7 +13150,7 @@
       </c>
       <c r="AZ59" s="8"/>
     </row>
-    <row r="60" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:52" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="4"/>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -13094,7 +13210,7 @@
       </c>
       <c r="AZ60" s="8"/>
     </row>
-    <row r="61" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="4"/>
       <c r="C61" s="53"/>
       <c r="D61" s="53"/>
@@ -13147,7 +13263,7 @@
       <c r="AY61" s="18"/>
       <c r="AZ61" s="8"/>
     </row>
-    <row r="62" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="4"/>
       <c r="C62" s="55"/>
       <c r="D62" s="55"/>
@@ -13200,7 +13316,7 @@
       <c r="AY62" s="36"/>
       <c r="AZ62" s="12"/>
     </row>
-    <row r="63" spans="2:52" ht="57" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:52" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="4"/>
       <c r="C63" s="53" t="s">
         <v>27</v>
@@ -13293,7 +13409,7 @@
       </c>
       <c r="AZ63" s="8"/>
     </row>
-    <row r="64" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="4"/>
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
@@ -13346,7 +13462,7 @@
       <c r="AY64" s="36"/>
       <c r="AZ64" s="8"/>
     </row>
-    <row r="65" spans="2:52" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:52" ht="63" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" s="4"/>
       <c r="C65" s="59" t="s">
         <v>34</v>
@@ -13437,7 +13553,7 @@
       </c>
       <c r="AZ65" s="8"/>
     </row>
-    <row r="66" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="4"/>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
@@ -13490,7 +13606,7 @@
       <c r="AY66" s="36"/>
       <c r="AZ66" s="8"/>
     </row>
-    <row r="67" spans="2:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="4"/>
       <c r="C67" s="59" t="s">
         <v>34</v>
@@ -13581,7 +13697,7 @@
       </c>
       <c r="AZ67" s="8"/>
     </row>
-    <row r="68" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="4"/>
       <c r="C68" s="55"/>
       <c r="D68" s="55"/>
@@ -13634,7 +13750,7 @@
       <c r="AY68" s="36"/>
       <c r="AZ68" s="8"/>
     </row>
-    <row r="69" spans="2:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:52" ht="47.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" s="4"/>
       <c r="C69" s="59" t="s">
         <v>34</v>
@@ -13725,7 +13841,7 @@
       </c>
       <c r="AZ69" s="8"/>
     </row>
-    <row r="70" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" s="37"/>
       <c r="C70" s="52"/>
       <c r="D70" s="52"/>
@@ -13778,7 +13894,7 @@
       <c r="AY70" s="38"/>
       <c r="AZ70" s="37"/>
     </row>
-    <row r="71" spans="2:52" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:52" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" s="4"/>
       <c r="C71" s="53"/>
       <c r="D71" s="53"/>
@@ -13843,7 +13959,7 @@
       </c>
       <c r="AZ71" s="12"/>
     </row>
-    <row r="72" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="4"/>
       <c r="C72" s="53"/>
       <c r="D72" s="53"/>
@@ -13896,7 +14012,7 @@
       <c r="AY72" s="17"/>
       <c r="AZ72" s="8"/>
     </row>
-    <row r="73" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="37"/>
       <c r="C73" s="52"/>
       <c r="D73" s="52"/>
@@ -13949,7 +14065,7 @@
       <c r="AY73" s="38"/>
       <c r="AZ73" s="37"/>
     </row>
-    <row r="74" spans="2:52" ht="114" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:52" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="4"/>
       <c r="C74" s="59" t="s">
         <v>34</v>
@@ -14048,7 +14164,7 @@
       </c>
       <c r="AZ74" s="12"/>
     </row>
-    <row r="75" spans="2:52" ht="28.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:52" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="4"/>
       <c r="C75" s="59" t="s">
         <v>34</v>
@@ -14143,7 +14259,7 @@
       <c r="AY75" s="17"/>
       <c r="AZ75" s="12"/>
     </row>
-    <row r="76" spans="2:52" ht="28.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:52" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="4"/>
       <c r="C76" s="59" t="s">
         <v>34</v>
@@ -14238,7 +14354,7 @@
       <c r="AY76" s="17"/>
       <c r="AZ76" s="12"/>
     </row>
-    <row r="77" spans="2:52" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:52" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" s="4"/>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
@@ -14295,7 +14411,7 @@
       <c r="AY77" s="17"/>
       <c r="AZ77" s="12"/>
     </row>
-    <row r="78" spans="2:52" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:52" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="4"/>
       <c r="C78" s="59" t="s">
         <v>34</v>
@@ -14394,7 +14510,7 @@
       <c r="AY78" s="17"/>
       <c r="AZ78" s="12"/>
     </row>
-    <row r="79" spans="2:52" collapsed="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:52" collapsed="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="4"/>
       <c r="C79" s="53"/>
       <c r="D79" s="53"/>
@@ -14447,7 +14563,7 @@
       <c r="AY79" s="17"/>
       <c r="AZ79" s="8"/>
     </row>
-    <row r="80" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" s="37"/>
       <c r="C80" s="52"/>
       <c r="D80" s="52"/>
@@ -14500,7 +14616,7 @@
       <c r="AY80" s="38"/>
       <c r="AZ80" s="37"/>
     </row>
-    <row r="81" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" s="4"/>
       <c r="C81" s="53"/>
       <c r="D81" s="53"/>
@@ -14599,7 +14715,7 @@
       </c>
       <c r="AZ81" s="8"/>
     </row>
-    <row r="82" spans="2:52" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" s="37"/>
       <c r="C82" s="52"/>
       <c r="D82" s="52"/>

</xml_diff>